<commit_message>
Fixing repeated trial bug
</commit_message>
<xml_diff>
--- a/notebooks/manual_data.xlsx
+++ b/notebooks/manual_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholasdevito/Documents/GitHub/covid_trials_tracker-covid/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7386EF-89CE-8745-8747-09DA4AA6B341}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23B5198-8C09-B74B-A98D-9B6A2805F28F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" activeTab="4" xr2:uid="{EB2E916D-92E5-6547-902E-71CC9B785F8F}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9111" uniqueCount="2817">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9109" uniqueCount="2817">
   <si>
     <t>unique_spon_names</t>
   </si>
@@ -13594,7 +13594,7 @@
   <dimension ref="A1:G890"/>
   <sheetViews>
     <sheetView topLeftCell="A864" workbookViewId="0">
-      <selection activeCell="E893" sqref="E893"/>
+      <selection activeCell="A889" sqref="A889"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31532,10 +31532,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ABCEDD8-99CD-E64D-83C4-23A5F7177A3C}">
-  <dimension ref="A1:C998"/>
+  <dimension ref="A1:C997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A722" workbookViewId="0">
+      <selection activeCell="A739" sqref="A739"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -39676,326 +39676,326 @@
     </row>
     <row r="740" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A740" s="6" t="s">
-        <v>2428</v>
+        <v>2030</v>
       </c>
       <c r="B740" s="8">
-        <v>43913</v>
+        <v>43982</v>
       </c>
       <c r="C740" s="8">
-        <v>43913</v>
+        <v>43982</v>
       </c>
     </row>
     <row r="741" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A741" s="6" t="s">
-        <v>2030</v>
+        <v>2020</v>
       </c>
       <c r="B741" s="8">
-        <v>43982</v>
+        <v>44044</v>
       </c>
       <c r="C741" s="8">
-        <v>43982</v>
+        <v>44136</v>
       </c>
     </row>
     <row r="742" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A742" s="6" t="s">
-        <v>2020</v>
+        <v>2097</v>
       </c>
       <c r="B742" s="8">
-        <v>44044</v>
+        <v>44275</v>
       </c>
       <c r="C742" s="8">
-        <v>44136</v>
+        <v>44640</v>
       </c>
     </row>
     <row r="743" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A743" s="6" t="s">
-        <v>2097</v>
+        <v>2018</v>
       </c>
       <c r="B743" s="8">
-        <v>44275</v>
+        <v>44307</v>
       </c>
       <c r="C743" s="8">
-        <v>44640</v>
+        <v>44429</v>
       </c>
     </row>
     <row r="744" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A744" s="6" t="s">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="B744" s="8">
-        <v>44307</v>
+        <v>44228</v>
       </c>
       <c r="C744" s="8">
-        <v>44429</v>
+        <v>44378</v>
       </c>
     </row>
     <row r="745" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A745" s="6" t="s">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="B745" s="8">
-        <v>44228</v>
+        <v>44073</v>
       </c>
       <c r="C745" s="8">
-        <v>44378</v>
+        <v>44073</v>
       </c>
     </row>
     <row r="746" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A746" s="6" t="s">
-        <v>2019</v>
+        <v>2031</v>
       </c>
       <c r="B746" s="8">
-        <v>44073</v>
+        <v>43970</v>
       </c>
       <c r="C746" s="8">
-        <v>44073</v>
+        <v>43970</v>
       </c>
     </row>
     <row r="747" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A747" s="6" t="s">
-        <v>2031</v>
+        <v>2024</v>
       </c>
       <c r="B747" s="8">
-        <v>43970</v>
+        <v>44012</v>
       </c>
       <c r="C747" s="8">
-        <v>43970</v>
+        <v>44073</v>
       </c>
     </row>
     <row r="748" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A748" s="6" t="s">
-        <v>2024</v>
+        <v>2038</v>
       </c>
       <c r="B748" s="8">
-        <v>44012</v>
+        <v>44135</v>
       </c>
       <c r="C748" s="8">
-        <v>44073</v>
+        <v>44286</v>
       </c>
     </row>
     <row r="749" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A749" s="6" t="s">
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="B749" s="8">
-        <v>44135</v>
+        <v>44196</v>
       </c>
       <c r="C749" s="8">
-        <v>44286</v>
+        <v>44211</v>
       </c>
     </row>
     <row r="750" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A750" s="6" t="s">
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="B750" s="8">
-        <v>44196</v>
+        <v>44012</v>
       </c>
       <c r="C750" s="8">
-        <v>44211</v>
+        <v>44073</v>
       </c>
     </row>
     <row r="751" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A751" s="6" t="s">
-        <v>2040</v>
+        <v>2025</v>
       </c>
       <c r="B751" s="8">
+        <v>43981</v>
+      </c>
+      <c r="C751" s="8">
         <v>44012</v>
-      </c>
-      <c r="C751" s="8">
-        <v>44073</v>
       </c>
     </row>
     <row r="752" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A752" s="6" t="s">
-        <v>2025</v>
+        <v>2098</v>
       </c>
       <c r="B752" s="8">
-        <v>43981</v>
+        <v>44075</v>
       </c>
       <c r="C752" s="8">
-        <v>44012</v>
+        <v>44075</v>
       </c>
     </row>
     <row r="753" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A753" s="6" t="s">
-        <v>2098</v>
+        <v>2026</v>
       </c>
       <c r="B753" s="8">
-        <v>44075</v>
+        <v>44348</v>
       </c>
       <c r="C753" s="8">
-        <v>44075</v>
+        <v>44348</v>
       </c>
     </row>
     <row r="754" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A754" s="6" t="s">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="B754" s="8">
-        <v>44348</v>
+        <v>42521</v>
       </c>
       <c r="C754" s="8">
-        <v>44348</v>
+        <v>43921</v>
       </c>
     </row>
     <row r="755" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A755" s="6" t="s">
-        <v>2027</v>
+        <v>2034</v>
       </c>
       <c r="B755" s="8">
-        <v>42521</v>
+        <v>44105</v>
       </c>
       <c r="C755" s="8">
-        <v>43921</v>
+        <v>44134</v>
       </c>
     </row>
     <row r="756" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A756" s="6" t="s">
-        <v>2034</v>
+        <v>2099</v>
       </c>
       <c r="B756" s="8">
-        <v>44105</v>
+        <v>43891</v>
       </c>
       <c r="C756" s="8">
-        <v>44134</v>
+        <v>43922</v>
       </c>
     </row>
     <row r="757" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A757" s="6" t="s">
-        <v>2099</v>
+        <v>2100</v>
       </c>
       <c r="B757" s="8">
-        <v>43891</v>
+        <v>43946</v>
       </c>
       <c r="C757" s="8">
-        <v>43922</v>
+        <v>43961</v>
       </c>
     </row>
     <row r="758" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A758" s="6" t="s">
-        <v>2100</v>
+        <v>2041</v>
       </c>
       <c r="B758" s="8">
-        <v>43946</v>
+        <v>44268</v>
       </c>
       <c r="C758" s="8">
-        <v>43961</v>
+        <v>44268</v>
       </c>
     </row>
     <row r="759" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A759" s="6" t="s">
-        <v>2041</v>
+        <v>2433</v>
       </c>
       <c r="B759" s="8">
-        <v>44268</v>
+        <v>44074</v>
       </c>
       <c r="C759" s="8">
-        <v>44268</v>
+        <v>44074</v>
       </c>
     </row>
     <row r="760" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A760" s="6" t="s">
-        <v>2433</v>
+        <v>2022</v>
       </c>
       <c r="B760" s="8">
-        <v>44074</v>
+        <v>43971</v>
       </c>
       <c r="C760" s="8">
-        <v>44074</v>
+        <v>43981</v>
       </c>
     </row>
     <row r="761" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A761" s="6" t="s">
-        <v>2022</v>
+        <v>2035</v>
       </c>
       <c r="B761" s="8">
-        <v>43971</v>
+        <v>44166</v>
       </c>
       <c r="C761" s="8">
-        <v>43981</v>
+        <v>44166</v>
       </c>
     </row>
     <row r="762" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A762" s="6" t="s">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="B762" s="8">
-        <v>44166</v>
+        <v>44104</v>
       </c>
       <c r="C762" s="8">
-        <v>44166</v>
+        <v>44104</v>
       </c>
     </row>
     <row r="763" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A763" s="6" t="s">
-        <v>2036</v>
+        <v>2050</v>
       </c>
       <c r="B763" s="8">
-        <v>44104</v>
+        <v>44316</v>
       </c>
       <c r="C763" s="8">
-        <v>44104</v>
+        <v>44316</v>
       </c>
     </row>
     <row r="764" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A764" s="6" t="s">
-        <v>2050</v>
+        <v>2023</v>
       </c>
       <c r="B764" s="8">
-        <v>44316</v>
+        <v>44926</v>
       </c>
       <c r="C764" s="8">
-        <v>44316</v>
+        <v>44927</v>
       </c>
     </row>
     <row r="765" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A765" s="6" t="s">
-        <v>2023</v>
+        <v>2051</v>
       </c>
       <c r="B765" s="8">
-        <v>44926</v>
+        <v>45382</v>
       </c>
       <c r="C765" s="8">
-        <v>44927</v>
+        <v>45382</v>
       </c>
     </row>
     <row r="766" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A766" s="6" t="s">
-        <v>2051</v>
+        <v>2037</v>
       </c>
       <c r="B766" s="8">
-        <v>45382</v>
+        <v>44109</v>
       </c>
       <c r="C766" s="8">
-        <v>45382</v>
+        <v>44144</v>
       </c>
     </row>
     <row r="767" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A767" s="6" t="s">
-        <v>2037</v>
+        <v>2052</v>
       </c>
       <c r="B767" s="8">
-        <v>44109</v>
+        <v>44013</v>
       </c>
       <c r="C767" s="8">
-        <v>44144</v>
+        <v>44075</v>
       </c>
     </row>
     <row r="768" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A768" s="6" t="s">
-        <v>2052</v>
+        <v>2053</v>
       </c>
       <c r="B768" s="8">
-        <v>44013</v>
+        <v>44282</v>
       </c>
       <c r="C768" s="8">
-        <v>44075</v>
+        <v>44561</v>
       </c>
     </row>
     <row r="769" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A769" s="6" t="s">
-        <v>2053</v>
+        <v>2044</v>
       </c>
       <c r="B769" s="8">
         <v>44282</v>
@@ -40006,1268 +40006,1262 @@
     </row>
     <row r="770" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A770" s="6" t="s">
-        <v>2044</v>
+        <v>2101</v>
       </c>
       <c r="B770" s="8">
-        <v>44282</v>
+        <v>43983</v>
       </c>
       <c r="C770" s="8">
-        <v>44561</v>
+        <v>44531</v>
       </c>
     </row>
     <row r="771" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A771" s="6" t="s">
-        <v>2101</v>
+        <v>2058</v>
       </c>
       <c r="B771" s="8">
-        <v>43983</v>
+        <v>44104</v>
       </c>
       <c r="C771" s="8">
-        <v>44531</v>
+        <v>44196</v>
       </c>
     </row>
     <row r="772" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A772" s="6" t="s">
-        <v>2058</v>
+        <v>2059</v>
       </c>
       <c r="B772" s="8">
-        <v>44104</v>
+        <v>43946</v>
       </c>
       <c r="C772" s="8">
-        <v>44196</v>
+        <v>43951</v>
       </c>
     </row>
     <row r="773" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A773" s="6" t="s">
-        <v>2059</v>
+        <v>2045</v>
       </c>
       <c r="B773" s="8">
-        <v>43946</v>
+        <v>44100</v>
       </c>
       <c r="C773" s="8">
-        <v>43951</v>
+        <v>44161</v>
       </c>
     </row>
     <row r="774" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A774" s="6" t="s">
-        <v>2045</v>
+        <v>2102</v>
       </c>
       <c r="B774" s="8">
-        <v>44100</v>
+        <v>44317</v>
       </c>
       <c r="C774" s="8">
-        <v>44161</v>
+        <v>44317</v>
       </c>
     </row>
     <row r="775" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A775" s="6" t="s">
-        <v>2102</v>
+        <v>2103</v>
       </c>
       <c r="B775" s="8">
-        <v>44317</v>
+        <v>44136</v>
       </c>
       <c r="C775" s="8">
-        <v>44317</v>
+        <v>44166</v>
       </c>
     </row>
     <row r="776" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A776" s="6" t="s">
-        <v>2103</v>
+        <v>2060</v>
       </c>
       <c r="B776" s="8">
-        <v>44136</v>
+        <v>43982</v>
       </c>
       <c r="C776" s="8">
-        <v>44166</v>
+        <v>44104</v>
       </c>
     </row>
     <row r="777" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A777" s="6" t="s">
-        <v>2060</v>
+        <v>2104</v>
       </c>
       <c r="B777" s="8">
-        <v>43982</v>
+        <v>44134</v>
       </c>
       <c r="C777" s="8">
-        <v>44104</v>
+        <v>44134</v>
       </c>
     </row>
     <row r="778" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A778" s="6" t="s">
-        <v>2104</v>
+        <v>2046</v>
       </c>
       <c r="B778" s="8">
-        <v>44134</v>
+        <v>44278</v>
       </c>
       <c r="C778" s="8">
-        <v>44134</v>
+        <v>44370</v>
       </c>
     </row>
     <row r="779" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A779" s="6" t="s">
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="B779" s="8">
-        <v>44278</v>
+        <v>44313</v>
       </c>
       <c r="C779" s="8">
-        <v>44370</v>
+        <v>44374</v>
       </c>
     </row>
     <row r="780" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A780" s="6" t="s">
-        <v>2047</v>
+        <v>2061</v>
       </c>
       <c r="B780" s="8">
-        <v>44313</v>
+        <v>44255</v>
       </c>
       <c r="C780" s="8">
-        <v>44374</v>
+        <v>44985</v>
       </c>
     </row>
     <row r="781" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A781" s="6" t="s">
-        <v>2061</v>
+        <v>2066</v>
       </c>
       <c r="B781" s="8">
-        <v>44255</v>
+        <v>44926</v>
       </c>
       <c r="C781" s="8">
-        <v>44985</v>
+        <v>44926</v>
       </c>
     </row>
     <row r="782" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A782" s="6" t="s">
-        <v>2066</v>
+        <v>2486</v>
       </c>
       <c r="B782" s="8">
-        <v>44926</v>
+        <v>44105</v>
       </c>
       <c r="C782" s="8">
-        <v>44926</v>
+        <v>44105</v>
       </c>
     </row>
     <row r="783" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A783" s="6" t="s">
-        <v>2486</v>
+        <v>2487</v>
       </c>
       <c r="B783" s="8">
-        <v>44105</v>
+        <v>44075</v>
       </c>
       <c r="C783" s="8">
-        <v>44105</v>
+        <v>44075</v>
       </c>
     </row>
     <row r="784" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A784" s="6" t="s">
-        <v>2487</v>
+        <v>2488</v>
       </c>
       <c r="B784" s="8">
-        <v>44075</v>
+        <v>43982</v>
       </c>
       <c r="C784" s="8">
-        <v>44075</v>
+        <v>44012</v>
       </c>
     </row>
     <row r="785" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A785" s="6" t="s">
-        <v>2488</v>
+        <v>2489</v>
       </c>
       <c r="B785" s="8">
-        <v>43982</v>
+        <v>44255</v>
       </c>
       <c r="C785" s="8">
-        <v>44012</v>
+        <v>44364</v>
       </c>
     </row>
     <row r="786" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A786" s="6" t="s">
-        <v>2489</v>
+        <v>2490</v>
       </c>
       <c r="B786" s="8">
-        <v>44255</v>
+        <v>44501</v>
       </c>
       <c r="C786" s="8">
-        <v>44364</v>
+        <v>44561</v>
       </c>
     </row>
     <row r="787" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A787" s="6" t="s">
-        <v>2490</v>
+        <v>2491</v>
       </c>
       <c r="B787" s="8">
-        <v>44501</v>
+        <v>44109</v>
       </c>
       <c r="C787" s="8">
-        <v>44561</v>
+        <v>44144</v>
       </c>
     </row>
     <row r="788" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A788" s="6" t="s">
-        <v>2491</v>
+        <v>2492</v>
       </c>
       <c r="B788" s="8">
-        <v>44109</v>
+        <v>44100</v>
       </c>
       <c r="C788" s="8">
-        <v>44144</v>
+        <v>44116</v>
       </c>
     </row>
     <row r="789" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A789" s="6" t="s">
-        <v>2492</v>
+        <v>2493</v>
       </c>
       <c r="B789" s="8">
-        <v>44100</v>
+        <v>44829</v>
       </c>
       <c r="C789" s="8">
-        <v>44116</v>
+        <v>44829</v>
       </c>
     </row>
     <row r="790" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A790" s="6" t="s">
-        <v>2493</v>
+        <v>2494</v>
       </c>
       <c r="B790" s="8">
-        <v>44829</v>
+        <v>44293</v>
       </c>
       <c r="C790" s="8">
-        <v>44829</v>
+        <v>44476</v>
       </c>
     </row>
     <row r="791" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A791" s="6" t="s">
-        <v>2494</v>
+        <v>2495</v>
       </c>
       <c r="B791" s="8">
-        <v>44293</v>
+        <v>44044</v>
       </c>
       <c r="C791" s="8">
-        <v>44476</v>
+        <v>44074</v>
       </c>
     </row>
     <row r="792" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A792" s="6" t="s">
-        <v>2495</v>
+        <v>2496</v>
       </c>
       <c r="B792" s="8">
-        <v>44044</v>
+        <v>43952</v>
       </c>
       <c r="C792" s="8">
-        <v>44074</v>
+        <v>43983</v>
       </c>
     </row>
     <row r="793" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A793" s="6" t="s">
-        <v>2496</v>
+        <v>2497</v>
       </c>
       <c r="B793" s="8">
-        <v>43952</v>
+        <v>44013</v>
       </c>
       <c r="C793" s="8">
-        <v>43983</v>
+        <v>44075</v>
       </c>
     </row>
     <row r="794" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A794" s="6" t="s">
-        <v>2497</v>
+        <v>2498</v>
       </c>
       <c r="B794" s="8">
-        <v>44013</v>
+        <v>44074</v>
       </c>
       <c r="C794" s="8">
-        <v>44075</v>
+        <v>44104</v>
       </c>
     </row>
     <row r="795" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A795" s="6" t="s">
-        <v>2498</v>
+        <v>2499</v>
       </c>
       <c r="B795" s="8">
-        <v>44074</v>
+        <v>44135</v>
       </c>
       <c r="C795" s="8">
-        <v>44104</v>
+        <v>44196</v>
       </c>
     </row>
     <row r="796" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A796" s="6" t="s">
-        <v>2499</v>
+        <v>2500</v>
       </c>
       <c r="B796" s="8">
-        <v>44135</v>
+        <v>44440</v>
       </c>
       <c r="C796" s="8">
-        <v>44196</v>
+        <v>44440</v>
       </c>
     </row>
     <row r="797" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A797" s="6" t="s">
-        <v>2500</v>
+        <v>2501</v>
       </c>
       <c r="B797" s="8">
-        <v>44440</v>
+        <v>44134</v>
       </c>
       <c r="C797" s="8">
-        <v>44440</v>
+        <v>44650</v>
       </c>
     </row>
     <row r="798" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A798" s="6" t="s">
-        <v>2501</v>
+        <v>2502</v>
       </c>
       <c r="B798" s="8">
-        <v>44134</v>
+        <v>43971</v>
       </c>
       <c r="C798" s="8">
-        <v>44650</v>
+        <v>44104</v>
       </c>
     </row>
     <row r="799" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A799" s="6" t="s">
-        <v>2502</v>
+        <v>2503</v>
       </c>
       <c r="B799" s="8">
-        <v>43971</v>
+        <v>44013</v>
       </c>
       <c r="C799" s="8">
-        <v>44104</v>
+        <v>44348</v>
       </c>
     </row>
     <row r="800" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A800" s="6" t="s">
-        <v>2503</v>
+        <v>2504</v>
       </c>
       <c r="B800" s="8">
-        <v>44013</v>
+        <v>44073</v>
       </c>
       <c r="C800" s="8">
-        <v>44348</v>
+        <v>44073</v>
       </c>
     </row>
     <row r="801" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A801" s="6" t="s">
-        <v>2504</v>
+        <v>2505</v>
       </c>
       <c r="B801" s="8">
-        <v>44073</v>
+        <v>46106</v>
       </c>
       <c r="C801" s="8">
-        <v>44073</v>
+        <v>46106</v>
       </c>
     </row>
     <row r="802" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A802" s="6" t="s">
-        <v>2505</v>
+        <v>2506</v>
       </c>
       <c r="B802" s="8">
-        <v>46106</v>
+        <v>44500</v>
       </c>
       <c r="C802" s="8">
-        <v>46106</v>
+        <v>44926</v>
       </c>
     </row>
     <row r="803" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A803" s="6" t="s">
-        <v>2506</v>
+        <v>2507</v>
       </c>
       <c r="B803" s="8">
-        <v>44500</v>
+        <v>43947</v>
       </c>
       <c r="C803" s="8">
-        <v>44926</v>
+        <v>43949</v>
       </c>
     </row>
     <row r="804" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A804" s="6" t="s">
-        <v>2507</v>
+        <v>2508</v>
       </c>
       <c r="B804" s="8">
-        <v>43947</v>
+        <v>44104</v>
       </c>
       <c r="C804" s="8">
-        <v>43949</v>
+        <v>44104</v>
       </c>
     </row>
     <row r="805" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A805" s="6" t="s">
-        <v>2508</v>
+        <v>2509</v>
       </c>
       <c r="B805" s="8">
-        <v>44104</v>
+        <v>43966</v>
       </c>
       <c r="C805" s="8">
-        <v>44104</v>
+        <v>43966</v>
       </c>
     </row>
     <row r="806" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A806" s="6" t="s">
-        <v>2509</v>
+        <v>2510</v>
       </c>
       <c r="B806" s="8">
-        <v>43966</v>
+        <v>44197</v>
       </c>
       <c r="C806" s="8">
-        <v>43966</v>
+        <v>44287</v>
       </c>
     </row>
     <row r="807" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A807" s="6" t="s">
-        <v>2510</v>
+        <v>2511</v>
       </c>
       <c r="B807" s="8">
-        <v>44197</v>
+        <v>44643</v>
       </c>
       <c r="C807" s="8">
-        <v>44287</v>
+        <v>44643</v>
       </c>
     </row>
     <row r="808" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A808" s="6" t="s">
-        <v>2511</v>
+        <v>2512</v>
       </c>
       <c r="B808" s="8">
-        <v>44643</v>
+        <v>43979</v>
       </c>
       <c r="C808" s="8">
-        <v>44643</v>
+        <v>44010</v>
       </c>
     </row>
     <row r="809" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A809" s="6" t="s">
-        <v>2512</v>
+        <v>2513</v>
       </c>
       <c r="B809" s="8">
-        <v>43979</v>
+        <v>44165</v>
       </c>
       <c r="C809" s="8">
-        <v>44010</v>
+        <v>44165</v>
       </c>
     </row>
     <row r="810" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A810" s="6" t="s">
-        <v>2513</v>
+        <v>2514</v>
       </c>
       <c r="B810" s="8">
-        <v>44165</v>
+        <v>44129</v>
       </c>
       <c r="C810" s="8">
-        <v>44165</v>
+        <v>44190</v>
       </c>
     </row>
     <row r="811" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A811" s="6" t="s">
-        <v>2514</v>
+        <v>2515</v>
       </c>
       <c r="B811" s="8">
-        <v>44129</v>
+        <v>43923</v>
       </c>
       <c r="C811" s="8">
-        <v>44190</v>
+        <v>43936</v>
       </c>
     </row>
     <row r="812" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A812" s="6" t="s">
-        <v>2515</v>
+        <v>2516</v>
       </c>
       <c r="B812" s="8">
-        <v>43923</v>
+        <v>44044</v>
       </c>
       <c r="C812" s="8">
-        <v>43936</v>
+        <v>44044</v>
       </c>
     </row>
     <row r="813" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A813" s="6" t="s">
-        <v>2516</v>
+        <v>2517</v>
       </c>
       <c r="B813" s="8">
-        <v>44044</v>
+        <v>43981</v>
       </c>
       <c r="C813" s="8">
-        <v>44044</v>
+        <v>44012</v>
       </c>
     </row>
     <row r="814" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A814" s="6" t="s">
-        <v>2517</v>
+        <v>2518</v>
       </c>
       <c r="B814" s="8">
-        <v>43981</v>
+        <v>44287</v>
       </c>
       <c r="C814" s="8">
-        <v>44012</v>
+        <v>44652</v>
       </c>
     </row>
     <row r="815" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A815" s="6" t="s">
-        <v>2518</v>
+        <v>2519</v>
       </c>
       <c r="B815" s="8">
-        <v>44287</v>
+        <v>44104</v>
       </c>
       <c r="C815" s="8">
-        <v>44652</v>
+        <v>44135</v>
       </c>
     </row>
     <row r="816" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A816" s="6" t="s">
-        <v>2519</v>
+        <v>2520</v>
       </c>
       <c r="B816" s="8">
-        <v>44104</v>
+        <v>43915</v>
       </c>
       <c r="C816" s="8">
-        <v>44135</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="817" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A817" s="6" t="s">
-        <v>2520</v>
+        <v>2521</v>
       </c>
       <c r="B817" s="8">
-        <v>43915</v>
+        <v>44012</v>
       </c>
       <c r="C817" s="8">
-        <v>43915</v>
+        <v>44042</v>
       </c>
     </row>
     <row r="818" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A818" s="6" t="s">
-        <v>2521</v>
+        <v>2522</v>
       </c>
       <c r="B818" s="8">
-        <v>44012</v>
+        <v>44592</v>
       </c>
       <c r="C818" s="8">
-        <v>44042</v>
+        <v>44651</v>
       </c>
     </row>
     <row r="819" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A819" s="6" t="s">
-        <v>2522</v>
+        <v>2523</v>
       </c>
       <c r="B819" s="8">
-        <v>44592</v>
+        <v>44011</v>
       </c>
       <c r="C819" s="8">
-        <v>44651</v>
+        <v>44376</v>
       </c>
     </row>
     <row r="820" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A820" s="6" t="s">
-        <v>2523</v>
+        <v>2524</v>
       </c>
       <c r="B820" s="8">
-        <v>44011</v>
+        <v>43982</v>
       </c>
       <c r="C820" s="8">
-        <v>44376</v>
+        <v>44012</v>
       </c>
     </row>
     <row r="821" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A821" s="6" t="s">
-        <v>2524</v>
+        <v>2525</v>
       </c>
       <c r="B821" s="8">
-        <v>43982</v>
+        <v>44043</v>
       </c>
       <c r="C821" s="8">
-        <v>44012</v>
+        <v>44074</v>
       </c>
     </row>
     <row r="822" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A822" s="6" t="s">
-        <v>2525</v>
+        <v>2526</v>
       </c>
       <c r="B822" s="8">
-        <v>44043</v>
+        <v>43971</v>
       </c>
       <c r="C822" s="8">
-        <v>44074</v>
+        <v>43971</v>
       </c>
     </row>
     <row r="823" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A823" s="6" t="s">
-        <v>2526</v>
+        <v>2527</v>
       </c>
       <c r="B823" s="8">
-        <v>43971</v>
+        <v>44196</v>
       </c>
       <c r="C823" s="8">
-        <v>43971</v>
+        <v>44561</v>
       </c>
     </row>
     <row r="824" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A824" s="6" t="s">
-        <v>2527</v>
+        <v>2528</v>
       </c>
       <c r="B824" s="8">
-        <v>44196</v>
+        <v>44287</v>
       </c>
       <c r="C824" s="8">
-        <v>44561</v>
+        <v>44531</v>
       </c>
     </row>
     <row r="825" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A825" s="6" t="s">
-        <v>2528</v>
+        <v>2529</v>
       </c>
       <c r="B825" s="8">
-        <v>44287</v>
+        <v>44285</v>
       </c>
       <c r="C825" s="8">
-        <v>44531</v>
+        <v>44650</v>
       </c>
     </row>
     <row r="826" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A826" s="6" t="s">
-        <v>2529</v>
+        <v>2530</v>
       </c>
       <c r="B826" s="8">
-        <v>44285</v>
+        <v>44272</v>
       </c>
       <c r="C826" s="8">
-        <v>44650</v>
+        <v>44637</v>
       </c>
     </row>
     <row r="827" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A827" s="6" t="s">
-        <v>2530</v>
+        <v>2531</v>
       </c>
       <c r="B827" s="8">
-        <v>44272</v>
+        <v>44227</v>
       </c>
       <c r="C827" s="8">
-        <v>44637</v>
+        <v>44256</v>
       </c>
     </row>
     <row r="828" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A828" s="6" t="s">
-        <v>2531</v>
+        <v>2532</v>
       </c>
       <c r="B828" s="8">
-        <v>44227</v>
+        <v>44141</v>
       </c>
       <c r="C828" s="8">
-        <v>44256</v>
+        <v>44141</v>
       </c>
     </row>
     <row r="829" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A829" s="6" t="s">
-        <v>2532</v>
+        <v>2533</v>
       </c>
       <c r="B829" s="8">
-        <v>44141</v>
+        <v>44682</v>
       </c>
       <c r="C829" s="8">
-        <v>44141</v>
+        <v>44682</v>
       </c>
     </row>
     <row r="830" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A830" s="6" t="s">
-        <v>2533</v>
+        <v>2534</v>
       </c>
       <c r="B830" s="8">
-        <v>44682</v>
+        <v>44012</v>
       </c>
       <c r="C830" s="8">
-        <v>44682</v>
+        <v>44104</v>
       </c>
     </row>
     <row r="831" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A831" s="6" t="s">
-        <v>2534</v>
+        <v>2535</v>
       </c>
       <c r="B831" s="8">
-        <v>44012</v>
+        <v>45748</v>
       </c>
       <c r="C831" s="8">
-        <v>44104</v>
+        <v>45748</v>
       </c>
     </row>
     <row r="832" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A832" s="6" t="s">
-        <v>2535</v>
+        <v>2536</v>
       </c>
       <c r="B832" s="8">
-        <v>45748</v>
+        <v>44075</v>
       </c>
       <c r="C832" s="8">
-        <v>45748</v>
+        <v>44166</v>
       </c>
     </row>
     <row r="833" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A833" s="6" t="s">
-        <v>2536</v>
+        <v>2537</v>
       </c>
       <c r="B833" s="8">
-        <v>44075</v>
+        <v>44638</v>
       </c>
       <c r="C833" s="8">
-        <v>44166</v>
+        <v>44699</v>
       </c>
     </row>
     <row r="834" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A834" s="6" t="s">
-        <v>2537</v>
+        <v>2538</v>
       </c>
       <c r="B834" s="8">
-        <v>44638</v>
+        <v>44013</v>
       </c>
       <c r="C834" s="8">
-        <v>44699</v>
+        <v>44013</v>
       </c>
     </row>
     <row r="835" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A835" s="6" t="s">
-        <v>2538</v>
+        <v>2539</v>
       </c>
       <c r="B835" s="8">
-        <v>44013</v>
+        <v>43921</v>
       </c>
       <c r="C835" s="8">
-        <v>44013</v>
+        <v>44043</v>
       </c>
     </row>
     <row r="836" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A836" s="6" t="s">
-        <v>2539</v>
+        <v>2540</v>
       </c>
       <c r="B836" s="8">
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="C836" s="8">
-        <v>44043</v>
+        <v>43922</v>
       </c>
     </row>
     <row r="837" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A837" s="6" t="s">
-        <v>2540</v>
+        <v>2541</v>
       </c>
       <c r="B837" s="8">
-        <v>43922</v>
+        <v>43941</v>
       </c>
       <c r="C837" s="8">
-        <v>43922</v>
+        <v>43971</v>
       </c>
     </row>
     <row r="838" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A838" s="6" t="s">
-        <v>2541</v>
+        <v>2542</v>
       </c>
       <c r="B838" s="8">
-        <v>43941</v>
+        <v>44643</v>
       </c>
       <c r="C838" s="8">
-        <v>43971</v>
+        <v>44643</v>
       </c>
     </row>
     <row r="839" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A839" s="6" t="s">
-        <v>2542</v>
+        <v>2543</v>
       </c>
       <c r="B839" s="8">
-        <v>44643</v>
+        <v>43931</v>
       </c>
       <c r="C839" s="8">
-        <v>44643</v>
+        <v>43951</v>
       </c>
     </row>
     <row r="840" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A840" s="6" t="s">
-        <v>2543</v>
+        <v>2544</v>
       </c>
       <c r="B840" s="8">
-        <v>43931</v>
+        <v>44104</v>
       </c>
       <c r="C840" s="8">
-        <v>43951</v>
+        <v>44196</v>
       </c>
     </row>
     <row r="841" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A841" s="6" t="s">
-        <v>2544</v>
+        <v>2545</v>
       </c>
       <c r="B841" s="8">
-        <v>44104</v>
+        <v>44166</v>
       </c>
       <c r="C841" s="8">
-        <v>44196</v>
+        <v>44166</v>
       </c>
     </row>
     <row r="842" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A842" s="6" t="s">
-        <v>2545</v>
+        <v>2546</v>
       </c>
       <c r="B842" s="8">
-        <v>44166</v>
+        <v>44134</v>
       </c>
       <c r="C842" s="8">
-        <v>44166</v>
+        <v>44227</v>
       </c>
     </row>
     <row r="843" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A843" s="6" t="s">
-        <v>2546</v>
+        <v>2547</v>
       </c>
       <c r="B843" s="8">
-        <v>44134</v>
+        <v>44013</v>
       </c>
       <c r="C843" s="8">
-        <v>44227</v>
+        <v>44166</v>
       </c>
     </row>
     <row r="844" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A844" s="6" t="s">
-        <v>2547</v>
+        <v>2548</v>
       </c>
       <c r="B844" s="8">
-        <v>44013</v>
+        <v>44286</v>
       </c>
       <c r="C844" s="8">
-        <v>44166</v>
+        <v>44561</v>
       </c>
     </row>
     <row r="845" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A845" s="6" t="s">
-        <v>2548</v>
+        <v>2549</v>
       </c>
       <c r="B845" s="8">
-        <v>44286</v>
+        <v>44107</v>
       </c>
       <c r="C845" s="8">
-        <v>44561</v>
+        <v>44134</v>
       </c>
     </row>
     <row r="846" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A846" s="6" t="s">
-        <v>2549</v>
-      </c>
-      <c r="B846" s="8">
-        <v>44107</v>
-      </c>
-      <c r="C846" s="8">
-        <v>44134</v>
+        <v>2550</v>
+      </c>
+      <c r="B846" s="6" t="s">
+        <v>2262</v>
+      </c>
+      <c r="C846" s="6" t="s">
+        <v>2262</v>
       </c>
     </row>
     <row r="847" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A847" s="6" t="s">
-        <v>2550</v>
-      </c>
-      <c r="B847" s="6" t="s">
-        <v>2262</v>
-      </c>
-      <c r="C847" s="6" t="s">
-        <v>2262</v>
+        <v>2551</v>
+      </c>
+      <c r="B847" s="8">
+        <v>44256</v>
+      </c>
+      <c r="C847" s="8">
+        <v>44256</v>
       </c>
     </row>
     <row r="848" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A848" s="6" t="s">
-        <v>2551</v>
+        <v>2552</v>
       </c>
       <c r="B848" s="8">
-        <v>44256</v>
+        <v>44347</v>
       </c>
       <c r="C848" s="8">
-        <v>44256</v>
+        <v>44712</v>
       </c>
     </row>
     <row r="849" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A849" s="6" t="s">
-        <v>2552</v>
+        <v>2553</v>
       </c>
       <c r="B849" s="8">
-        <v>44347</v>
+        <v>44986</v>
       </c>
       <c r="C849" s="8">
-        <v>44712</v>
+        <v>44986</v>
       </c>
     </row>
     <row r="850" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A850" s="6" t="s">
-        <v>2553</v>
+        <v>2554</v>
       </c>
       <c r="B850" s="8">
-        <v>44986</v>
+        <v>44013</v>
       </c>
       <c r="C850" s="8">
-        <v>44986</v>
+        <v>44013</v>
       </c>
     </row>
     <row r="851" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A851" s="6" t="s">
-        <v>2554</v>
+        <v>2555</v>
       </c>
       <c r="B851" s="8">
-        <v>44013</v>
+        <v>44075</v>
       </c>
       <c r="C851" s="8">
-        <v>44013</v>
+        <v>44105</v>
       </c>
     </row>
     <row r="852" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A852" s="6" t="s">
-        <v>2555</v>
+        <v>2556</v>
       </c>
       <c r="B852" s="8">
-        <v>44075</v>
+        <v>44042</v>
       </c>
       <c r="C852" s="8">
-        <v>44105</v>
+        <v>44407</v>
       </c>
     </row>
     <row r="853" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A853" s="6" t="s">
-        <v>2556</v>
+        <v>2557</v>
       </c>
       <c r="B853" s="8">
-        <v>44042</v>
+        <v>44074</v>
       </c>
       <c r="C853" s="8">
-        <v>44407</v>
+        <v>44196</v>
       </c>
     </row>
     <row r="854" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A854" s="6" t="s">
-        <v>2557</v>
+        <v>2558</v>
       </c>
       <c r="B854" s="8">
-        <v>44074</v>
+        <v>43981</v>
       </c>
       <c r="C854" s="8">
-        <v>44196</v>
+        <v>43997</v>
       </c>
     </row>
     <row r="855" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A855" s="6" t="s">
-        <v>2558</v>
+        <v>2559</v>
       </c>
       <c r="B855" s="8">
-        <v>43981</v>
+        <v>44074</v>
       </c>
       <c r="C855" s="8">
-        <v>43997</v>
+        <v>44196</v>
       </c>
     </row>
     <row r="856" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A856" s="6" t="s">
-        <v>2559</v>
+        <v>2560</v>
       </c>
       <c r="B856" s="8">
-        <v>44074</v>
+        <v>44196</v>
       </c>
       <c r="C856" s="8">
-        <v>44196</v>
+        <v>44286</v>
       </c>
     </row>
     <row r="857" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A857" s="6" t="s">
-        <v>2560</v>
+        <v>2561</v>
       </c>
       <c r="B857" s="8">
-        <v>44196</v>
+        <v>44287</v>
       </c>
       <c r="C857" s="8">
-        <v>44286</v>
+        <v>44378</v>
       </c>
     </row>
     <row r="858" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A858" s="6" t="s">
-        <v>2561</v>
+        <v>2562</v>
       </c>
       <c r="B858" s="8">
-        <v>44287</v>
+        <v>44042</v>
       </c>
       <c r="C858" s="8">
-        <v>44378</v>
+        <v>44042</v>
       </c>
     </row>
     <row r="859" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A859" s="6" t="s">
-        <v>2562</v>
+        <v>2563</v>
       </c>
       <c r="B859" s="8">
-        <v>44042</v>
+        <v>44926</v>
       </c>
       <c r="C859" s="8">
-        <v>44042</v>
+        <v>44926</v>
       </c>
     </row>
     <row r="860" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A860" s="6" t="s">
-        <v>2563</v>
+        <v>2564</v>
       </c>
       <c r="B860" s="8">
-        <v>44926</v>
+        <v>44185</v>
       </c>
       <c r="C860" s="8">
-        <v>44926</v>
+        <v>44316</v>
       </c>
     </row>
     <row r="861" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A861" s="6" t="s">
-        <v>2564</v>
+        <v>2565</v>
       </c>
       <c r="B861" s="8">
-        <v>44185</v>
+        <v>44285</v>
       </c>
       <c r="C861" s="8">
-        <v>44316</v>
+        <v>44285</v>
       </c>
     </row>
     <row r="862" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A862" s="6" t="s">
-        <v>2565</v>
+        <v>2566</v>
       </c>
       <c r="B862" s="8">
-        <v>44285</v>
+        <v>44135</v>
       </c>
       <c r="C862" s="8">
-        <v>44285</v>
+        <v>44196</v>
       </c>
     </row>
     <row r="863" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A863" s="6" t="s">
-        <v>2566</v>
+        <v>2567</v>
       </c>
       <c r="B863" s="8">
-        <v>44135</v>
+        <v>43988</v>
       </c>
       <c r="C863" s="8">
-        <v>44196</v>
+        <v>44018</v>
       </c>
     </row>
     <row r="864" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A864" s="6" t="s">
-        <v>2567</v>
+        <v>2568</v>
       </c>
       <c r="B864" s="8">
-        <v>43988</v>
+        <v>44075</v>
       </c>
       <c r="C864" s="8">
-        <v>44018</v>
+        <v>44256</v>
       </c>
     </row>
     <row r="865" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A865" s="6" t="s">
-        <v>2568</v>
+        <v>2569</v>
       </c>
       <c r="B865" s="8">
-        <v>44075</v>
+        <v>43983</v>
       </c>
       <c r="C865" s="8">
-        <v>44256</v>
+        <v>44089</v>
       </c>
     </row>
     <row r="866" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A866" s="6" t="s">
-        <v>2569</v>
+        <v>2570</v>
       </c>
       <c r="B866" s="8">
-        <v>43983</v>
+        <v>44287</v>
       </c>
       <c r="C866" s="8">
-        <v>44089</v>
+        <v>44531</v>
       </c>
     </row>
     <row r="867" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A867" s="6" t="s">
-        <v>2570</v>
+        <v>2571</v>
       </c>
       <c r="B867" s="8">
-        <v>44287</v>
+        <v>43952</v>
       </c>
       <c r="C867" s="8">
-        <v>44531</v>
+        <v>43952</v>
       </c>
     </row>
     <row r="868" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A868" s="6" t="s">
-        <v>2571</v>
+        <v>2572</v>
       </c>
       <c r="B868" s="8">
-        <v>43952</v>
+        <v>44105</v>
       </c>
       <c r="C868" s="8">
-        <v>43952</v>
+        <v>44136</v>
       </c>
     </row>
     <row r="869" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A869" s="6" t="s">
-        <v>2572</v>
+        <v>2573</v>
       </c>
       <c r="B869" s="8">
-        <v>44105</v>
+        <v>44228</v>
       </c>
       <c r="C869" s="8">
-        <v>44136</v>
+        <v>44228</v>
       </c>
     </row>
     <row r="870" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A870" s="6" t="s">
-        <v>2573</v>
+        <v>2574</v>
       </c>
       <c r="B870" s="8">
-        <v>44228</v>
+        <v>44075</v>
       </c>
       <c r="C870" s="8">
-        <v>44228</v>
+        <v>44075</v>
       </c>
     </row>
     <row r="871" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A871" s="6" t="s">
-        <v>2574</v>
+        <v>2575</v>
       </c>
       <c r="B871" s="8">
-        <v>44075</v>
+        <v>44012</v>
       </c>
       <c r="C871" s="8">
-        <v>44075</v>
+        <v>44561</v>
       </c>
     </row>
     <row r="872" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A872" s="6" t="s">
-        <v>2575</v>
+        <v>2576</v>
       </c>
       <c r="B872" s="8">
-        <v>44012</v>
+        <v>43983</v>
       </c>
       <c r="C872" s="8">
-        <v>44561</v>
+        <v>44044</v>
       </c>
     </row>
     <row r="873" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A873" s="6" t="s">
-        <v>2576</v>
+        <v>2577</v>
       </c>
       <c r="B873" s="8">
-        <v>43983</v>
+        <v>44105</v>
       </c>
       <c r="C873" s="8">
-        <v>44044</v>
+        <v>44105</v>
       </c>
     </row>
     <row r="874" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A874" s="6" t="s">
-        <v>2577</v>
+        <v>2578</v>
       </c>
       <c r="B874" s="8">
-        <v>44105</v>
+        <v>44012</v>
       </c>
       <c r="C874" s="8">
-        <v>44105</v>
+        <v>44012</v>
       </c>
     </row>
     <row r="875" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A875" s="6" t="s">
-        <v>2578</v>
+        <v>2579</v>
       </c>
       <c r="B875" s="8">
-        <v>44012</v>
+        <v>43983</v>
       </c>
       <c r="C875" s="8">
-        <v>44012</v>
+        <v>43983</v>
       </c>
     </row>
     <row r="876" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A876" s="6" t="s">
-        <v>2579</v>
-      </c>
-      <c r="B876" s="8">
-        <v>43983</v>
+        <v>900</v>
+      </c>
+      <c r="B876" s="6" t="s">
+        <v>2262</v>
       </c>
       <c r="C876" s="8">
-        <v>43983</v>
+        <v>44059</v>
       </c>
     </row>
     <row r="877" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A877" s="6" t="s">
-        <v>900</v>
+        <v>2081</v>
       </c>
       <c r="B877" s="6" t="s">
         <v>2262</v>
       </c>
       <c r="C877" s="8">
-        <v>44059</v>
+        <v>44462</v>
       </c>
     </row>
     <row r="878" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A878" s="6" t="s">
-        <v>2081</v>
+        <v>2580</v>
       </c>
       <c r="B878" s="6" t="s">
         <v>2262</v>
       </c>
       <c r="C878" s="8">
-        <v>44462</v>
+        <v>43919</v>
       </c>
     </row>
     <row r="879" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A879" s="6" t="s">
-        <v>2580</v>
+        <v>2581</v>
       </c>
       <c r="B879" s="6" t="s">
         <v>2262</v>
       </c>
       <c r="C879" s="8">
-        <v>43919</v>
+        <v>44196</v>
       </c>
     </row>
     <row r="880" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A880" s="6" t="s">
-        <v>2581</v>
+        <v>2582</v>
       </c>
       <c r="B880" s="6" t="s">
         <v>2262</v>
       </c>
       <c r="C880" s="8">
-        <v>44196</v>
+        <v>44298</v>
       </c>
     </row>
     <row r="881" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A881" s="6" t="s">
-        <v>2582</v>
+        <v>2583</v>
       </c>
       <c r="B881" s="6" t="s">
         <v>2262</v>
       </c>
       <c r="C881" s="8">
-        <v>44298</v>
+        <v>44012</v>
       </c>
     </row>
     <row r="882" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A882" s="6" t="s">
-        <v>2583</v>
-      </c>
-      <c r="B882" s="6" t="s">
-        <v>2262</v>
+        <v>822</v>
+      </c>
+      <c r="B882" s="8">
+        <v>43935</v>
       </c>
       <c r="C882" s="8">
-        <v>44012</v>
+        <v>43935</v>
       </c>
     </row>
     <row r="883" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A883" s="6" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="B883" s="8">
-        <v>43935</v>
+        <v>43921</v>
       </c>
       <c r="C883" s="8">
-        <v>43935</v>
+        <v>43921</v>
       </c>
     </row>
     <row r="884" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A884" s="6" t="s">
-        <v>824</v>
-      </c>
-      <c r="B884" s="8">
-        <v>43921</v>
-      </c>
-      <c r="C884" s="8">
-        <v>43921</v>
-      </c>
+      <c r="A884" s="6"/>
+      <c r="B884" s="6"/>
+      <c r="C884" s="6"/>
     </row>
     <row r="885" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A885" s="6"/>
@@ -41833,11 +41827,6 @@
       <c r="A997" s="6"/>
       <c r="B997" s="6"/>
       <c r="C997" s="6"/>
-    </row>
-    <row r="998" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A998" s="6"/>
-      <c r="B998" s="6"/>
-      <c r="C998" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -41846,10 +41835,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F8C4E0-02D7-BD4E-9875-A292DA5969FB}">
-  <dimension ref="A1:D998"/>
+  <dimension ref="A1:D997"/>
   <sheetViews>
-    <sheetView topLeftCell="A528" workbookViewId="0">
-      <selection activeCell="C543" sqref="C543"/>
+    <sheetView topLeftCell="A722" workbookViewId="0">
+      <selection activeCell="A739" sqref="A739"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -47948,7 +47937,7 @@
     </row>
     <row r="740" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A740" s="6" t="s">
-        <v>2428</v>
+        <v>2030</v>
       </c>
       <c r="B740" s="13"/>
       <c r="C740" s="13"/>
@@ -47956,7 +47945,7 @@
     </row>
     <row r="741" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A741" s="6" t="s">
-        <v>2030</v>
+        <v>2020</v>
       </c>
       <c r="B741" s="13"/>
       <c r="C741" s="13"/>
@@ -47964,7 +47953,7 @@
     </row>
     <row r="742" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A742" s="6" t="s">
-        <v>2020</v>
+        <v>2097</v>
       </c>
       <c r="B742" s="13"/>
       <c r="C742" s="13"/>
@@ -47972,7 +47961,7 @@
     </row>
     <row r="743" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A743" s="6" t="s">
-        <v>2097</v>
+        <v>2018</v>
       </c>
       <c r="B743" s="13"/>
       <c r="C743" s="13"/>
@@ -47980,7 +47969,7 @@
     </row>
     <row r="744" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A744" s="6" t="s">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="B744" s="13"/>
       <c r="C744" s="13"/>
@@ -47988,7 +47977,7 @@
     </row>
     <row r="745" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A745" s="6" t="s">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="B745" s="13"/>
       <c r="C745" s="13"/>
@@ -47996,29 +47985,29 @@
     </row>
     <row r="746" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A746" s="6" t="s">
-        <v>2019</v>
-      </c>
-      <c r="B746" s="13"/>
-      <c r="C746" s="13"/>
-      <c r="D746" s="13"/>
+        <v>2031</v>
+      </c>
+      <c r="B746" s="11" t="s">
+        <v>2288</v>
+      </c>
+      <c r="C746" s="8">
+        <v>43924</v>
+      </c>
+      <c r="D746" s="13" t="s">
+        <v>2265</v>
+      </c>
     </row>
     <row r="747" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A747" s="6" t="s">
-        <v>2031</v>
-      </c>
-      <c r="B747" s="11" t="s">
-        <v>2288</v>
-      </c>
-      <c r="C747" s="8">
-        <v>43924</v>
-      </c>
-      <c r="D747" s="13" t="s">
-        <v>2265</v>
-      </c>
+        <v>2024</v>
+      </c>
+      <c r="B747" s="13"/>
+      <c r="C747" s="13"/>
+      <c r="D747" s="13"/>
     </row>
     <row r="748" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A748" s="6" t="s">
-        <v>2024</v>
+        <v>2038</v>
       </c>
       <c r="B748" s="13"/>
       <c r="C748" s="13"/>
@@ -48026,7 +48015,7 @@
     </row>
     <row r="749" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A749" s="6" t="s">
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="B749" s="13"/>
       <c r="C749" s="13"/>
@@ -48034,7 +48023,7 @@
     </row>
     <row r="750" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A750" s="6" t="s">
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="B750" s="13"/>
       <c r="C750" s="13"/>
@@ -48042,7 +48031,7 @@
     </row>
     <row r="751" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A751" s="6" t="s">
-        <v>2040</v>
+        <v>2025</v>
       </c>
       <c r="B751" s="13"/>
       <c r="C751" s="13"/>
@@ -48050,7 +48039,7 @@
     </row>
     <row r="752" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A752" s="6" t="s">
-        <v>2025</v>
+        <v>2098</v>
       </c>
       <c r="B752" s="13"/>
       <c r="C752" s="13"/>
@@ -48058,7 +48047,7 @@
     </row>
     <row r="753" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A753" s="6" t="s">
-        <v>2098</v>
+        <v>2026</v>
       </c>
       <c r="B753" s="13"/>
       <c r="C753" s="13"/>
@@ -48066,7 +48055,7 @@
     </row>
     <row r="754" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A754" s="6" t="s">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="B754" s="13"/>
       <c r="C754" s="13"/>
@@ -48074,7 +48063,7 @@
     </row>
     <row r="755" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A755" s="6" t="s">
-        <v>2027</v>
+        <v>2034</v>
       </c>
       <c r="B755" s="13"/>
       <c r="C755" s="13"/>
@@ -48082,7 +48071,7 @@
     </row>
     <row r="756" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A756" s="6" t="s">
-        <v>2034</v>
+        <v>2099</v>
       </c>
       <c r="B756" s="13"/>
       <c r="C756" s="13"/>
@@ -48090,7 +48079,7 @@
     </row>
     <row r="757" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A757" s="6" t="s">
-        <v>2099</v>
+        <v>2100</v>
       </c>
       <c r="B757" s="13"/>
       <c r="C757" s="13"/>
@@ -48098,7 +48087,7 @@
     </row>
     <row r="758" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A758" s="6" t="s">
-        <v>2100</v>
+        <v>2041</v>
       </c>
       <c r="B758" s="13"/>
       <c r="C758" s="13"/>
@@ -48106,29 +48095,29 @@
     </row>
     <row r="759" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A759" s="6" t="s">
-        <v>2041</v>
-      </c>
-      <c r="B759" s="13"/>
-      <c r="C759" s="13"/>
-      <c r="D759" s="13"/>
+        <v>2433</v>
+      </c>
+      <c r="B759" s="11" t="s">
+        <v>2588</v>
+      </c>
+      <c r="C759" s="8">
+        <v>43932</v>
+      </c>
+      <c r="D759" s="13" t="s">
+        <v>2265</v>
+      </c>
     </row>
     <row r="760" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A760" s="6" t="s">
-        <v>2433</v>
-      </c>
-      <c r="B760" s="11" t="s">
-        <v>2588</v>
-      </c>
-      <c r="C760" s="8">
-        <v>43932</v>
-      </c>
-      <c r="D760" s="13" t="s">
-        <v>2265</v>
-      </c>
+        <v>2022</v>
+      </c>
+      <c r="B760" s="13"/>
+      <c r="C760" s="13"/>
+      <c r="D760" s="13"/>
     </row>
     <row r="761" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A761" s="6" t="s">
-        <v>2022</v>
+        <v>2035</v>
       </c>
       <c r="B761" s="13"/>
       <c r="C761" s="13"/>
@@ -48136,7 +48125,7 @@
     </row>
     <row r="762" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A762" s="6" t="s">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="B762" s="13"/>
       <c r="C762" s="13"/>
@@ -48144,7 +48133,7 @@
     </row>
     <row r="763" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A763" s="6" t="s">
-        <v>2036</v>
+        <v>2050</v>
       </c>
       <c r="B763" s="13"/>
       <c r="C763" s="13"/>
@@ -48152,7 +48141,7 @@
     </row>
     <row r="764" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A764" s="6" t="s">
-        <v>2050</v>
+        <v>2023</v>
       </c>
       <c r="B764" s="13"/>
       <c r="C764" s="13"/>
@@ -48160,7 +48149,7 @@
     </row>
     <row r="765" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A765" s="6" t="s">
-        <v>2023</v>
+        <v>2051</v>
       </c>
       <c r="B765" s="13"/>
       <c r="C765" s="13"/>
@@ -48168,7 +48157,7 @@
     </row>
     <row r="766" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A766" s="6" t="s">
-        <v>2051</v>
+        <v>2037</v>
       </c>
       <c r="B766" s="13"/>
       <c r="C766" s="13"/>
@@ -48176,7 +48165,7 @@
     </row>
     <row r="767" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A767" s="6" t="s">
-        <v>2037</v>
+        <v>2052</v>
       </c>
       <c r="B767" s="13"/>
       <c r="C767" s="13"/>
@@ -48184,7 +48173,7 @@
     </row>
     <row r="768" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A768" s="6" t="s">
-        <v>2052</v>
+        <v>2053</v>
       </c>
       <c r="B768" s="13"/>
       <c r="C768" s="13"/>
@@ -48192,7 +48181,7 @@
     </row>
     <row r="769" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A769" s="6" t="s">
-        <v>2053</v>
+        <v>2044</v>
       </c>
       <c r="B769" s="13"/>
       <c r="C769" s="13"/>
@@ -48200,7 +48189,7 @@
     </row>
     <row r="770" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A770" s="6" t="s">
-        <v>2044</v>
+        <v>2101</v>
       </c>
       <c r="B770" s="13"/>
       <c r="C770" s="13"/>
@@ -48208,7 +48197,7 @@
     </row>
     <row r="771" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A771" s="6" t="s">
-        <v>2101</v>
+        <v>2058</v>
       </c>
       <c r="B771" s="13"/>
       <c r="C771" s="13"/>
@@ -48216,7 +48205,7 @@
     </row>
     <row r="772" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A772" s="6" t="s">
-        <v>2058</v>
+        <v>2059</v>
       </c>
       <c r="B772" s="13"/>
       <c r="C772" s="13"/>
@@ -48224,7 +48213,7 @@
     </row>
     <row r="773" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A773" s="6" t="s">
-        <v>2059</v>
+        <v>2045</v>
       </c>
       <c r="B773" s="13"/>
       <c r="C773" s="13"/>
@@ -48232,7 +48221,7 @@
     </row>
     <row r="774" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A774" s="6" t="s">
-        <v>2045</v>
+        <v>2102</v>
       </c>
       <c r="B774" s="13"/>
       <c r="C774" s="13"/>
@@ -48240,7 +48229,7 @@
     </row>
     <row r="775" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A775" s="6" t="s">
-        <v>2102</v>
+        <v>2103</v>
       </c>
       <c r="B775" s="13"/>
       <c r="C775" s="13"/>
@@ -48248,7 +48237,7 @@
     </row>
     <row r="776" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A776" s="6" t="s">
-        <v>2103</v>
+        <v>2060</v>
       </c>
       <c r="B776" s="13"/>
       <c r="C776" s="13"/>
@@ -48256,7 +48245,7 @@
     </row>
     <row r="777" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A777" s="6" t="s">
-        <v>2060</v>
+        <v>2104</v>
       </c>
       <c r="B777" s="13"/>
       <c r="C777" s="13"/>
@@ -48264,7 +48253,7 @@
     </row>
     <row r="778" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A778" s="6" t="s">
-        <v>2104</v>
+        <v>2046</v>
       </c>
       <c r="B778" s="13"/>
       <c r="C778" s="13"/>
@@ -48272,7 +48261,7 @@
     </row>
     <row r="779" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A779" s="6" t="s">
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="B779" s="13"/>
       <c r="C779" s="13"/>
@@ -48280,7 +48269,7 @@
     </row>
     <row r="780" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A780" s="6" t="s">
-        <v>2047</v>
+        <v>2061</v>
       </c>
       <c r="B780" s="13"/>
       <c r="C780" s="13"/>
@@ -48288,7 +48277,7 @@
     </row>
     <row r="781" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A781" s="6" t="s">
-        <v>2061</v>
+        <v>2066</v>
       </c>
       <c r="B781" s="13"/>
       <c r="C781" s="13"/>
@@ -48296,7 +48285,7 @@
     </row>
     <row r="782" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A782" s="6" t="s">
-        <v>2066</v>
+        <v>2486</v>
       </c>
       <c r="B782" s="13"/>
       <c r="C782" s="13"/>
@@ -48304,7 +48293,7 @@
     </row>
     <row r="783" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A783" s="6" t="s">
-        <v>2486</v>
+        <v>2487</v>
       </c>
       <c r="B783" s="13"/>
       <c r="C783" s="13"/>
@@ -48312,7 +48301,7 @@
     </row>
     <row r="784" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A784" s="6" t="s">
-        <v>2487</v>
+        <v>2488</v>
       </c>
       <c r="B784" s="13"/>
       <c r="C784" s="13"/>
@@ -48320,7 +48309,7 @@
     </row>
     <row r="785" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A785" s="6" t="s">
-        <v>2488</v>
+        <v>2489</v>
       </c>
       <c r="B785" s="13"/>
       <c r="C785" s="13"/>
@@ -48328,7 +48317,7 @@
     </row>
     <row r="786" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A786" s="6" t="s">
-        <v>2489</v>
+        <v>2490</v>
       </c>
       <c r="B786" s="13"/>
       <c r="C786" s="13"/>
@@ -48336,7 +48325,7 @@
     </row>
     <row r="787" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A787" s="6" t="s">
-        <v>2490</v>
+        <v>2491</v>
       </c>
       <c r="B787" s="13"/>
       <c r="C787" s="13"/>
@@ -48344,7 +48333,7 @@
     </row>
     <row r="788" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A788" s="6" t="s">
-        <v>2491</v>
+        <v>2492</v>
       </c>
       <c r="B788" s="13"/>
       <c r="C788" s="13"/>
@@ -48352,7 +48341,7 @@
     </row>
     <row r="789" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A789" s="6" t="s">
-        <v>2492</v>
+        <v>2493</v>
       </c>
       <c r="B789" s="13"/>
       <c r="C789" s="13"/>
@@ -48360,7 +48349,7 @@
     </row>
     <row r="790" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A790" s="6" t="s">
-        <v>2493</v>
+        <v>2494</v>
       </c>
       <c r="B790" s="13"/>
       <c r="C790" s="13"/>
@@ -48368,7 +48357,7 @@
     </row>
     <row r="791" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A791" s="6" t="s">
-        <v>2494</v>
+        <v>2495</v>
       </c>
       <c r="B791" s="13"/>
       <c r="C791" s="13"/>
@@ -48376,7 +48365,7 @@
     </row>
     <row r="792" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A792" s="6" t="s">
-        <v>2495</v>
+        <v>2496</v>
       </c>
       <c r="B792" s="13"/>
       <c r="C792" s="13"/>
@@ -48384,7 +48373,7 @@
     </row>
     <row r="793" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A793" s="6" t="s">
-        <v>2496</v>
+        <v>2497</v>
       </c>
       <c r="B793" s="13"/>
       <c r="C793" s="13"/>
@@ -48392,7 +48381,7 @@
     </row>
     <row r="794" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A794" s="6" t="s">
-        <v>2497</v>
+        <v>2498</v>
       </c>
       <c r="B794" s="13"/>
       <c r="C794" s="13"/>
@@ -48400,7 +48389,7 @@
     </row>
     <row r="795" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A795" s="6" t="s">
-        <v>2498</v>
+        <v>2499</v>
       </c>
       <c r="B795" s="13"/>
       <c r="C795" s="13"/>
@@ -48408,7 +48397,7 @@
     </row>
     <row r="796" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A796" s="6" t="s">
-        <v>2499</v>
+        <v>2500</v>
       </c>
       <c r="B796" s="13"/>
       <c r="C796" s="13"/>
@@ -48416,7 +48405,7 @@
     </row>
     <row r="797" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A797" s="6" t="s">
-        <v>2500</v>
+        <v>2501</v>
       </c>
       <c r="B797" s="13"/>
       <c r="C797" s="13"/>
@@ -48424,7 +48413,7 @@
     </row>
     <row r="798" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A798" s="6" t="s">
-        <v>2501</v>
+        <v>2502</v>
       </c>
       <c r="B798" s="13"/>
       <c r="C798" s="13"/>
@@ -48432,7 +48421,7 @@
     </row>
     <row r="799" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A799" s="6" t="s">
-        <v>2502</v>
+        <v>2503</v>
       </c>
       <c r="B799" s="13"/>
       <c r="C799" s="13"/>
@@ -48440,7 +48429,7 @@
     </row>
     <row r="800" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A800" s="6" t="s">
-        <v>2503</v>
+        <v>2504</v>
       </c>
       <c r="B800" s="13"/>
       <c r="C800" s="13"/>
@@ -48448,7 +48437,7 @@
     </row>
     <row r="801" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A801" s="6" t="s">
-        <v>2504</v>
+        <v>2505</v>
       </c>
       <c r="B801" s="13"/>
       <c r="C801" s="13"/>
@@ -48456,7 +48445,7 @@
     </row>
     <row r="802" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A802" s="6" t="s">
-        <v>2505</v>
+        <v>2506</v>
       </c>
       <c r="B802" s="13"/>
       <c r="C802" s="13"/>
@@ -48464,7 +48453,7 @@
     </row>
     <row r="803" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A803" s="6" t="s">
-        <v>2506</v>
+        <v>2507</v>
       </c>
       <c r="B803" s="13"/>
       <c r="C803" s="13"/>
@@ -48472,7 +48461,7 @@
     </row>
     <row r="804" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A804" s="6" t="s">
-        <v>2507</v>
+        <v>2508</v>
       </c>
       <c r="B804" s="13"/>
       <c r="C804" s="13"/>
@@ -48480,7 +48469,7 @@
     </row>
     <row r="805" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A805" s="6" t="s">
-        <v>2508</v>
+        <v>2509</v>
       </c>
       <c r="B805" s="13"/>
       <c r="C805" s="13"/>
@@ -48488,7 +48477,7 @@
     </row>
     <row r="806" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A806" s="6" t="s">
-        <v>2509</v>
+        <v>2510</v>
       </c>
       <c r="B806" s="13"/>
       <c r="C806" s="13"/>
@@ -48496,7 +48485,7 @@
     </row>
     <row r="807" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A807" s="6" t="s">
-        <v>2510</v>
+        <v>2511</v>
       </c>
       <c r="B807" s="13"/>
       <c r="C807" s="13"/>
@@ -48504,7 +48493,7 @@
     </row>
     <row r="808" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A808" s="6" t="s">
-        <v>2511</v>
+        <v>2512</v>
       </c>
       <c r="B808" s="13"/>
       <c r="C808" s="13"/>
@@ -48512,7 +48501,7 @@
     </row>
     <row r="809" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A809" s="6" t="s">
-        <v>2512</v>
+        <v>2513</v>
       </c>
       <c r="B809" s="13"/>
       <c r="C809" s="13"/>
@@ -48520,7 +48509,7 @@
     </row>
     <row r="810" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A810" s="6" t="s">
-        <v>2513</v>
+        <v>2514</v>
       </c>
       <c r="B810" s="13"/>
       <c r="C810" s="13"/>
@@ -48528,7 +48517,7 @@
     </row>
     <row r="811" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A811" s="6" t="s">
-        <v>2514</v>
+        <v>2515</v>
       </c>
       <c r="B811" s="13"/>
       <c r="C811" s="13"/>
@@ -48536,7 +48525,7 @@
     </row>
     <row r="812" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A812" s="6" t="s">
-        <v>2515</v>
+        <v>2516</v>
       </c>
       <c r="B812" s="13"/>
       <c r="C812" s="13"/>
@@ -48544,7 +48533,7 @@
     </row>
     <row r="813" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A813" s="6" t="s">
-        <v>2516</v>
+        <v>2517</v>
       </c>
       <c r="B813" s="13"/>
       <c r="C813" s="13"/>
@@ -48552,7 +48541,7 @@
     </row>
     <row r="814" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A814" s="6" t="s">
-        <v>2517</v>
+        <v>2518</v>
       </c>
       <c r="B814" s="13"/>
       <c r="C814" s="13"/>
@@ -48560,7 +48549,7 @@
     </row>
     <row r="815" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A815" s="6" t="s">
-        <v>2518</v>
+        <v>2519</v>
       </c>
       <c r="B815" s="13"/>
       <c r="C815" s="13"/>
@@ -48568,7 +48557,7 @@
     </row>
     <row r="816" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A816" s="6" t="s">
-        <v>2519</v>
+        <v>2520</v>
       </c>
       <c r="B816" s="13"/>
       <c r="C816" s="13"/>
@@ -48576,7 +48565,7 @@
     </row>
     <row r="817" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A817" s="6" t="s">
-        <v>2520</v>
+        <v>2521</v>
       </c>
       <c r="B817" s="13"/>
       <c r="C817" s="13"/>
@@ -48584,7 +48573,7 @@
     </row>
     <row r="818" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A818" s="6" t="s">
-        <v>2521</v>
+        <v>2522</v>
       </c>
       <c r="B818" s="13"/>
       <c r="C818" s="13"/>
@@ -48592,7 +48581,7 @@
     </row>
     <row r="819" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A819" s="6" t="s">
-        <v>2522</v>
+        <v>2523</v>
       </c>
       <c r="B819" s="13"/>
       <c r="C819" s="13"/>
@@ -48600,7 +48589,7 @@
     </row>
     <row r="820" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A820" s="6" t="s">
-        <v>2523</v>
+        <v>2524</v>
       </c>
       <c r="B820" s="13"/>
       <c r="C820" s="13"/>
@@ -48608,7 +48597,7 @@
     </row>
     <row r="821" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A821" s="6" t="s">
-        <v>2524</v>
+        <v>2525</v>
       </c>
       <c r="B821" s="13"/>
       <c r="C821" s="13"/>
@@ -48616,7 +48605,7 @@
     </row>
     <row r="822" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A822" s="6" t="s">
-        <v>2525</v>
+        <v>2526</v>
       </c>
       <c r="B822" s="13"/>
       <c r="C822" s="13"/>
@@ -48624,7 +48613,7 @@
     </row>
     <row r="823" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A823" s="6" t="s">
-        <v>2526</v>
+        <v>2527</v>
       </c>
       <c r="B823" s="13"/>
       <c r="C823" s="13"/>
@@ -48632,7 +48621,7 @@
     </row>
     <row r="824" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A824" s="6" t="s">
-        <v>2527</v>
+        <v>2528</v>
       </c>
       <c r="B824" s="13"/>
       <c r="C824" s="13"/>
@@ -48640,7 +48629,7 @@
     </row>
     <row r="825" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A825" s="6" t="s">
-        <v>2528</v>
+        <v>2529</v>
       </c>
       <c r="B825" s="13"/>
       <c r="C825" s="13"/>
@@ -48648,7 +48637,7 @@
     </row>
     <row r="826" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A826" s="6" t="s">
-        <v>2529</v>
+        <v>2530</v>
       </c>
       <c r="B826" s="13"/>
       <c r="C826" s="13"/>
@@ -48656,7 +48645,7 @@
     </row>
     <row r="827" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A827" s="6" t="s">
-        <v>2530</v>
+        <v>2531</v>
       </c>
       <c r="B827" s="13"/>
       <c r="C827" s="13"/>
@@ -48664,7 +48653,7 @@
     </row>
     <row r="828" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A828" s="6" t="s">
-        <v>2531</v>
+        <v>2532</v>
       </c>
       <c r="B828" s="13"/>
       <c r="C828" s="13"/>
@@ -48672,7 +48661,7 @@
     </row>
     <row r="829" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A829" s="6" t="s">
-        <v>2532</v>
+        <v>2533</v>
       </c>
       <c r="B829" s="13"/>
       <c r="C829" s="13"/>
@@ -48680,7 +48669,7 @@
     </row>
     <row r="830" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A830" s="6" t="s">
-        <v>2533</v>
+        <v>2534</v>
       </c>
       <c r="B830" s="13"/>
       <c r="C830" s="13"/>
@@ -48688,7 +48677,7 @@
     </row>
     <row r="831" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A831" s="6" t="s">
-        <v>2534</v>
+        <v>2535</v>
       </c>
       <c r="B831" s="13"/>
       <c r="C831" s="13"/>
@@ -48696,7 +48685,7 @@
     </row>
     <row r="832" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A832" s="6" t="s">
-        <v>2535</v>
+        <v>2536</v>
       </c>
       <c r="B832" s="13"/>
       <c r="C832" s="13"/>
@@ -48704,7 +48693,7 @@
     </row>
     <row r="833" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A833" s="6" t="s">
-        <v>2536</v>
+        <v>2537</v>
       </c>
       <c r="B833" s="13"/>
       <c r="C833" s="13"/>
@@ -48712,7 +48701,7 @@
     </row>
     <row r="834" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A834" s="6" t="s">
-        <v>2537</v>
+        <v>2538</v>
       </c>
       <c r="B834" s="13"/>
       <c r="C834" s="13"/>
@@ -48720,7 +48709,7 @@
     </row>
     <row r="835" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A835" s="6" t="s">
-        <v>2538</v>
+        <v>2539</v>
       </c>
       <c r="B835" s="13"/>
       <c r="C835" s="13"/>
@@ -48728,7 +48717,7 @@
     </row>
     <row r="836" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A836" s="6" t="s">
-        <v>2539</v>
+        <v>2540</v>
       </c>
       <c r="B836" s="13"/>
       <c r="C836" s="13"/>
@@ -48736,7 +48725,7 @@
     </row>
     <row r="837" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A837" s="6" t="s">
-        <v>2540</v>
+        <v>2541</v>
       </c>
       <c r="B837" s="13"/>
       <c r="C837" s="13"/>
@@ -48744,7 +48733,7 @@
     </row>
     <row r="838" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A838" s="6" t="s">
-        <v>2541</v>
+        <v>2542</v>
       </c>
       <c r="B838" s="13"/>
       <c r="C838" s="13"/>
@@ -48752,7 +48741,7 @@
     </row>
     <row r="839" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A839" s="6" t="s">
-        <v>2542</v>
+        <v>2543</v>
       </c>
       <c r="B839" s="13"/>
       <c r="C839" s="13"/>
@@ -48760,7 +48749,7 @@
     </row>
     <row r="840" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A840" s="6" t="s">
-        <v>2543</v>
+        <v>2544</v>
       </c>
       <c r="B840" s="13"/>
       <c r="C840" s="13"/>
@@ -48768,7 +48757,7 @@
     </row>
     <row r="841" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A841" s="6" t="s">
-        <v>2544</v>
+        <v>2545</v>
       </c>
       <c r="B841" s="13"/>
       <c r="C841" s="13"/>
@@ -48776,7 +48765,7 @@
     </row>
     <row r="842" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A842" s="6" t="s">
-        <v>2545</v>
+        <v>2546</v>
       </c>
       <c r="B842" s="13"/>
       <c r="C842" s="13"/>
@@ -48784,7 +48773,7 @@
     </row>
     <row r="843" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A843" s="6" t="s">
-        <v>2546</v>
+        <v>2547</v>
       </c>
       <c r="B843" s="13"/>
       <c r="C843" s="13"/>
@@ -48792,7 +48781,7 @@
     </row>
     <row r="844" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A844" s="6" t="s">
-        <v>2547</v>
+        <v>2548</v>
       </c>
       <c r="B844" s="13"/>
       <c r="C844" s="13"/>
@@ -48800,7 +48789,7 @@
     </row>
     <row r="845" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A845" s="6" t="s">
-        <v>2548</v>
+        <v>2549</v>
       </c>
       <c r="B845" s="13"/>
       <c r="C845" s="13"/>
@@ -48808,7 +48797,7 @@
     </row>
     <row r="846" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A846" s="6" t="s">
-        <v>2549</v>
+        <v>2550</v>
       </c>
       <c r="B846" s="13"/>
       <c r="C846" s="13"/>
@@ -48816,7 +48805,7 @@
     </row>
     <row r="847" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A847" s="6" t="s">
-        <v>2550</v>
+        <v>2551</v>
       </c>
       <c r="B847" s="13"/>
       <c r="C847" s="13"/>
@@ -48824,7 +48813,7 @@
     </row>
     <row r="848" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A848" s="6" t="s">
-        <v>2551</v>
+        <v>2552</v>
       </c>
       <c r="B848" s="13"/>
       <c r="C848" s="13"/>
@@ -48832,7 +48821,7 @@
     </row>
     <row r="849" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A849" s="6" t="s">
-        <v>2552</v>
+        <v>2553</v>
       </c>
       <c r="B849" s="13"/>
       <c r="C849" s="13"/>
@@ -48840,7 +48829,7 @@
     </row>
     <row r="850" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A850" s="6" t="s">
-        <v>2553</v>
+        <v>2554</v>
       </c>
       <c r="B850" s="13"/>
       <c r="C850" s="13"/>
@@ -48848,7 +48837,7 @@
     </row>
     <row r="851" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A851" s="6" t="s">
-        <v>2554</v>
+        <v>2555</v>
       </c>
       <c r="B851" s="13"/>
       <c r="C851" s="13"/>
@@ -48856,7 +48845,7 @@
     </row>
     <row r="852" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A852" s="6" t="s">
-        <v>2555</v>
+        <v>2556</v>
       </c>
       <c r="B852" s="13"/>
       <c r="C852" s="13"/>
@@ -48864,7 +48853,7 @@
     </row>
     <row r="853" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A853" s="6" t="s">
-        <v>2556</v>
+        <v>2557</v>
       </c>
       <c r="B853" s="13"/>
       <c r="C853" s="13"/>
@@ -48872,7 +48861,7 @@
     </row>
     <row r="854" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A854" s="6" t="s">
-        <v>2557</v>
+        <v>2558</v>
       </c>
       <c r="B854" s="13"/>
       <c r="C854" s="13"/>
@@ -48880,7 +48869,7 @@
     </row>
     <row r="855" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A855" s="6" t="s">
-        <v>2558</v>
+        <v>2559</v>
       </c>
       <c r="B855" s="13"/>
       <c r="C855" s="13"/>
@@ -48888,7 +48877,7 @@
     </row>
     <row r="856" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A856" s="6" t="s">
-        <v>2559</v>
+        <v>2560</v>
       </c>
       <c r="B856" s="13"/>
       <c r="C856" s="13"/>
@@ -48896,7 +48885,7 @@
     </row>
     <row r="857" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A857" s="6" t="s">
-        <v>2560</v>
+        <v>2561</v>
       </c>
       <c r="B857" s="13"/>
       <c r="C857" s="13"/>
@@ -48904,7 +48893,7 @@
     </row>
     <row r="858" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A858" s="6" t="s">
-        <v>2561</v>
+        <v>2562</v>
       </c>
       <c r="B858" s="13"/>
       <c r="C858" s="13"/>
@@ -48912,7 +48901,7 @@
     </row>
     <row r="859" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A859" s="6" t="s">
-        <v>2562</v>
+        <v>2563</v>
       </c>
       <c r="B859" s="13"/>
       <c r="C859" s="13"/>
@@ -48920,7 +48909,7 @@
     </row>
     <row r="860" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A860" s="6" t="s">
-        <v>2563</v>
+        <v>2564</v>
       </c>
       <c r="B860" s="13"/>
       <c r="C860" s="13"/>
@@ -48928,7 +48917,7 @@
     </row>
     <row r="861" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A861" s="6" t="s">
-        <v>2564</v>
+        <v>2565</v>
       </c>
       <c r="B861" s="13"/>
       <c r="C861" s="13"/>
@@ -48936,7 +48925,7 @@
     </row>
     <row r="862" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A862" s="6" t="s">
-        <v>2565</v>
+        <v>2566</v>
       </c>
       <c r="B862" s="13"/>
       <c r="C862" s="13"/>
@@ -48944,7 +48933,7 @@
     </row>
     <row r="863" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A863" s="6" t="s">
-        <v>2566</v>
+        <v>2567</v>
       </c>
       <c r="B863" s="13"/>
       <c r="C863" s="13"/>
@@ -48952,7 +48941,7 @@
     </row>
     <row r="864" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A864" s="6" t="s">
-        <v>2567</v>
+        <v>2568</v>
       </c>
       <c r="B864" s="13"/>
       <c r="C864" s="13"/>
@@ -48960,7 +48949,7 @@
     </row>
     <row r="865" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A865" s="6" t="s">
-        <v>2568</v>
+        <v>2569</v>
       </c>
       <c r="B865" s="13"/>
       <c r="C865" s="13"/>
@@ -48968,7 +48957,7 @@
     </row>
     <row r="866" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A866" s="6" t="s">
-        <v>2569</v>
+        <v>2570</v>
       </c>
       <c r="B866" s="13"/>
       <c r="C866" s="13"/>
@@ -48976,7 +48965,7 @@
     </row>
     <row r="867" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A867" s="6" t="s">
-        <v>2570</v>
+        <v>2571</v>
       </c>
       <c r="B867" s="13"/>
       <c r="C867" s="13"/>
@@ -48984,7 +48973,7 @@
     </row>
     <row r="868" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A868" s="6" t="s">
-        <v>2571</v>
+        <v>2572</v>
       </c>
       <c r="B868" s="13"/>
       <c r="C868" s="13"/>
@@ -48992,7 +48981,7 @@
     </row>
     <row r="869" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A869" s="6" t="s">
-        <v>2572</v>
+        <v>2573</v>
       </c>
       <c r="B869" s="13"/>
       <c r="C869" s="13"/>
@@ -49000,7 +48989,7 @@
     </row>
     <row r="870" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A870" s="6" t="s">
-        <v>2573</v>
+        <v>2574</v>
       </c>
       <c r="B870" s="13"/>
       <c r="C870" s="13"/>
@@ -49008,7 +48997,7 @@
     </row>
     <row r="871" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A871" s="6" t="s">
-        <v>2574</v>
+        <v>2575</v>
       </c>
       <c r="B871" s="13"/>
       <c r="C871" s="13"/>
@@ -49016,7 +49005,7 @@
     </row>
     <row r="872" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A872" s="6" t="s">
-        <v>2575</v>
+        <v>2576</v>
       </c>
       <c r="B872" s="13"/>
       <c r="C872" s="13"/>
@@ -49024,7 +49013,7 @@
     </row>
     <row r="873" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A873" s="6" t="s">
-        <v>2576</v>
+        <v>2577</v>
       </c>
       <c r="B873" s="13"/>
       <c r="C873" s="13"/>
@@ -49032,7 +49021,7 @@
     </row>
     <row r="874" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A874" s="6" t="s">
-        <v>2577</v>
+        <v>2578</v>
       </c>
       <c r="B874" s="13"/>
       <c r="C874" s="13"/>
@@ -49040,7 +49029,7 @@
     </row>
     <row r="875" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A875" s="6" t="s">
-        <v>2578</v>
+        <v>2579</v>
       </c>
       <c r="B875" s="13"/>
       <c r="C875" s="13"/>
@@ -49048,7 +49037,7 @@
     </row>
     <row r="876" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A876" s="6" t="s">
-        <v>2579</v>
+        <v>900</v>
       </c>
       <c r="B876" s="13"/>
       <c r="C876" s="13"/>
@@ -49056,7 +49045,7 @@
     </row>
     <row r="877" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A877" s="6" t="s">
-        <v>900</v>
+        <v>2081</v>
       </c>
       <c r="B877" s="13"/>
       <c r="C877" s="13"/>
@@ -49064,7 +49053,7 @@
     </row>
     <row r="878" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A878" s="6" t="s">
-        <v>2081</v>
+        <v>2580</v>
       </c>
       <c r="B878" s="13"/>
       <c r="C878" s="13"/>
@@ -49072,7 +49061,7 @@
     </row>
     <row r="879" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A879" s="6" t="s">
-        <v>2580</v>
+        <v>2581</v>
       </c>
       <c r="B879" s="13"/>
       <c r="C879" s="13"/>
@@ -49080,7 +49069,7 @@
     </row>
     <row r="880" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A880" s="6" t="s">
-        <v>2581</v>
+        <v>2582</v>
       </c>
       <c r="B880" s="13"/>
       <c r="C880" s="13"/>
@@ -49088,7 +49077,7 @@
     </row>
     <row r="881" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A881" s="6" t="s">
-        <v>2582</v>
+        <v>2583</v>
       </c>
       <c r="B881" s="13"/>
       <c r="C881" s="13"/>
@@ -49096,7 +49085,7 @@
     </row>
     <row r="882" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A882" s="6" t="s">
-        <v>2583</v>
+        <v>822</v>
       </c>
       <c r="B882" s="13"/>
       <c r="C882" s="13"/>
@@ -49104,29 +49093,27 @@
     </row>
     <row r="883" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A883" s="6" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="B883" s="13"/>
       <c r="C883" s="13"/>
-      <c r="D883" s="13"/>
     </row>
     <row r="884" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A884" s="6" t="s">
-        <v>824</v>
-      </c>
-      <c r="B884" s="13"/>
-      <c r="C884" s="13"/>
+      <c r="A884" s="6"/>
+      <c r="B884" s="6"/>
+      <c r="C884" s="6"/>
+      <c r="D884" s="6"/>
     </row>
     <row r="885" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A885" s="6"/>
       <c r="B885" s="6"/>
       <c r="C885" s="6"/>
-      <c r="D885" s="6"/>
     </row>
     <row r="886" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A886" s="6"/>
       <c r="B886" s="6"/>
       <c r="C886" s="6"/>
+      <c r="D886" s="6"/>
     </row>
     <row r="887" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A887" s="6"/>
@@ -49793,12 +49780,6 @@
       <c r="B997" s="6"/>
       <c r="C997" s="6"/>
       <c r="D997" s="6"/>
-    </row>
-    <row r="998" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A998" s="6"/>
-      <c r="B998" s="6"/>
-      <c r="C998" s="6"/>
-      <c r="D998" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -49830,8 +49811,8 @@
     <hyperlink ref="B652" r:id="rId26" xr:uid="{90603235-F868-F045-BD34-792CEE6E91F6}"/>
     <hyperlink ref="B657" r:id="rId27" xr:uid="{96D82271-D605-6445-A0C9-4F3F8ED6A2BB}"/>
     <hyperlink ref="B739" r:id="rId28" xr:uid="{AD1B15C8-8236-C849-A27C-78316AF8F3D6}"/>
-    <hyperlink ref="B747" r:id="rId29" xr:uid="{4FE241A4-E3F1-214C-B015-A237207CA726}"/>
-    <hyperlink ref="B760" r:id="rId30" xr:uid="{43EF46C9-1F6F-F246-9CF0-9743DB6796D7}"/>
+    <hyperlink ref="B746" r:id="rId29" xr:uid="{4FE241A4-E3F1-214C-B015-A237207CA726}"/>
+    <hyperlink ref="B759" r:id="rId30" xr:uid="{43EF46C9-1F6F-F246-9CF0-9743DB6796D7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Correcting figures and data
The interventions graph was not categorising correctly with the changes. Updated and graph replaced. Also a fix to a stray entry in the intervention data.
</commit_message>
<xml_diff>
--- a/notebooks/manual_data.xlsx
+++ b/notebooks/manual_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholasdevito/Documents/GitHub/covid_trials_tracker-covid/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F68EEA-2303-E54F-8B4F-C9EB56179D4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5854C7D6-EA84-874B-8D3B-B87C1E90418B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2420" yWindow="460" windowWidth="24520" windowHeight="14280" activeTab="1" xr2:uid="{EB2E916D-92E5-6547-902E-71CC9B785F8F}"/>
   </bookViews>
@@ -16904,8 +16904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC06582-2DEF-3F4C-9BDF-F5E9FA92249B}">
   <dimension ref="A1:F1092"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A462" workbookViewId="0">
-      <selection activeCell="B307" sqref="B307"/>
+    <sheetView tabSelected="1" topLeftCell="A730" workbookViewId="0">
+      <selection activeCell="D738" sqref="D738"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -29572,7 +29572,7 @@
         <v>2594</v>
       </c>
       <c r="C738" s="13" t="s">
-        <v>3503</v>
+        <v>1058</v>
       </c>
       <c r="D738" s="3" t="s">
         <v>2687</v>

</xml_diff>

<commit_message>
Fix merge bug for results section
Updates data and website with fix
</commit_message>
<xml_diff>
--- a/notebooks/manual_data.xlsx
+++ b/notebooks/manual_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholasdevito/Documents/GitHub/covid_trials_tracker-covid/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5854C7D6-EA84-874B-8D3B-B87C1E90418B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8946E4-578B-B449-AF22-3AD2460D2970}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="460" windowWidth="24520" windowHeight="14280" activeTab="1" xr2:uid="{EB2E916D-92E5-6547-902E-71CC9B785F8F}"/>
+    <workbookView xWindow="2420" yWindow="460" windowWidth="24520" windowHeight="14280" activeTab="3" xr2:uid="{EB2E916D-92E5-6547-902E-71CC9B785F8F}"/>
   </bookViews>
   <sheets>
     <sheet name="sponsor" sheetId="1" r:id="rId1"/>
@@ -16904,7 +16904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC06582-2DEF-3F4C-9BDF-F5E9FA92249B}">
   <dimension ref="A1:F1092"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A730" workbookViewId="0">
+    <sheetView topLeftCell="A688" workbookViewId="0">
       <selection activeCell="D738" sqref="D738"/>
     </sheetView>
   </sheetViews>
@@ -47587,8 +47587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F8C4E0-02D7-BD4E-9875-A292DA5969FB}">
   <dimension ref="A1:D997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -47596,7 +47596,7 @@
     <col min="1" max="1" width="37.33203125" customWidth="1"/>
     <col min="2" max="2" width="40.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="26.1640625" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -47607,10 +47607,10 @@
         <v>2734</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>2735</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>2736</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>2735</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Re-doing initial data cleaning
Inputting new data. Updateing data cleaning code. Some new cross-registration data.
</commit_message>
<xml_diff>
--- a/notebooks/manual_data.xlsx
+++ b/notebooks/manual_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholasdevito/Documents/GitHub/covid_trials_tracker-covid/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8946E4-578B-B449-AF22-3AD2460D2970}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A43E22E-68B0-F44A-872B-CB8FF1A92435}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="460" windowWidth="24520" windowHeight="14280" activeTab="3" xr2:uid="{EB2E916D-92E5-6547-902E-71CC9B785F8F}"/>
+    <workbookView xWindow="-260" yWindow="1240" windowWidth="24520" windowHeight="14280" activeTab="4" xr2:uid="{EB2E916D-92E5-6547-902E-71CC9B785F8F}"/>
   </bookViews>
   <sheets>
     <sheet name="sponsor" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9057" uniqueCount="3541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9072" uniqueCount="3547">
   <si>
     <t>unique_spon_names</t>
   </si>
@@ -10682,6 +10682,25 @@
   </si>
   <si>
     <t>Correspondence</t>
+  </si>
+  <si>
+    <t>EUCTR2020-001320-34</t>
+  </si>
+  <si>
+    <t>EUCTR2020-001320-34-NL</t>
+  </si>
+  <si>
+    <t>Phase 4</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Drug: Valsartan (Diovan)
+Drug: Placebo oral tablet</t>
+  </si>
+  <si>
+    <t>https://clinicaltrials.gov/ct2/show/NCT04335786</t>
   </si>
 </sst>
 </file>
@@ -10758,7 +10777,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -10786,7 +10805,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -15254,7 +15272,7 @@
       <c r="A517" t="s">
         <v>300</v>
       </c>
-      <c r="B517" s="18" t="s">
+      <c r="B517" s="17" t="s">
         <v>293</v>
       </c>
     </row>
@@ -16486,7 +16504,7 @@
       <c r="A671" t="s">
         <v>2920</v>
       </c>
-      <c r="B671" s="18" t="s">
+      <c r="B671" s="17" t="s">
         <v>2950</v>
       </c>
     </row>
@@ -22282,19 +22300,19 @@
       </c>
     </row>
     <row r="311" spans="1:6" ht="43" x14ac:dyDescent="0.2">
-      <c r="A311" s="20" t="s">
+      <c r="A311" s="19" t="s">
         <v>636</v>
       </c>
-      <c r="B311" s="20" t="s">
+      <c r="B311" s="19" t="s">
         <v>1349</v>
       </c>
-      <c r="C311" s="20" t="s">
+      <c r="C311" s="19" t="s">
         <v>3531</v>
       </c>
-      <c r="D311" s="20" t="s">
-        <v>1127</v>
-      </c>
-      <c r="E311" s="20" t="s">
+      <c r="D311" s="19" t="s">
+        <v>1127</v>
+      </c>
+      <c r="E311" s="19" t="s">
         <v>1127</v>
       </c>
       <c r="F311" s="2" t="s">
@@ -22302,19 +22320,19 @@
       </c>
     </row>
     <row r="312" spans="1:6" ht="29" x14ac:dyDescent="0.2">
-      <c r="A312" s="20" t="s">
+      <c r="A312" s="19" t="s">
         <v>638</v>
       </c>
-      <c r="B312" s="20" t="s">
+      <c r="B312" s="19" t="s">
         <v>1351</v>
       </c>
-      <c r="C312" s="20" t="s">
+      <c r="C312" s="19" t="s">
         <v>3531</v>
       </c>
-      <c r="D312" s="20" t="s">
-        <v>1127</v>
-      </c>
-      <c r="E312" s="20" t="s">
+      <c r="D312" s="19" t="s">
+        <v>1127</v>
+      </c>
+      <c r="E312" s="19" t="s">
         <v>1127</v>
       </c>
       <c r="F312" s="2" t="s">
@@ -29701,19 +29719,19 @@
       </c>
     </row>
     <row r="746" spans="1:5" ht="29" x14ac:dyDescent="0.2">
-      <c r="A746" s="19" t="s">
+      <c r="A746" s="18" t="s">
         <v>2514</v>
       </c>
-      <c r="B746" s="20" t="s">
+      <c r="B746" s="19" t="s">
         <v>2577</v>
       </c>
-      <c r="C746" s="19" t="s">
+      <c r="C746" s="18" t="s">
         <v>3457</v>
       </c>
-      <c r="D746" s="20" t="s">
-        <v>1127</v>
-      </c>
-      <c r="E746" s="20" t="s">
+      <c r="D746" s="19" t="s">
+        <v>1127</v>
+      </c>
+      <c r="E746" s="19" t="s">
         <v>1127</v>
       </c>
     </row>
@@ -29826,7 +29844,7 @@
       <c r="B753" s="3" t="s">
         <v>1535</v>
       </c>
-      <c r="C753" s="19" t="s">
+      <c r="C753" s="18" t="s">
         <v>3457</v>
       </c>
       <c r="D753" s="3" t="s">
@@ -47587,7 +47605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F8C4E0-02D7-BD4E-9875-A292DA5969FB}">
   <dimension ref="A1:D997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -47603,7 +47621,7 @@
       <c r="A1" s="7" t="s">
         <v>2202</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>2734</v>
       </c>
       <c r="C1" s="7" t="s">
@@ -53901,9 +53919,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2897C11-45D0-1143-9B66-314A64F11CA5}">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -54311,7 +54331,7 @@
       <c r="K8" t="s">
         <v>2646</v>
       </c>
-      <c r="L8" s="17" t="s">
+      <c r="L8" t="s">
         <v>2739</v>
       </c>
       <c r="M8">
@@ -54361,7 +54381,7 @@
       <c r="K9" t="s">
         <v>2549</v>
       </c>
-      <c r="L9" s="17" t="s">
+      <c r="L9" t="s">
         <v>2741</v>
       </c>
       <c r="M9">
@@ -54524,15 +54544,66 @@
         <v>43936</v>
       </c>
     </row>
+    <row r="13" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>3222</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1797</v>
+      </c>
+      <c r="C13" s="4">
+        <v>43923</v>
+      </c>
+      <c r="D13" s="4">
+        <v>43922</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2776</v>
+      </c>
+      <c r="F13" t="s">
+        <v>2874</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1798</v>
+      </c>
+      <c r="H13" t="s">
+        <v>3543</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1800</v>
+      </c>
+      <c r="J13" t="s">
+        <v>3544</v>
+      </c>
+      <c r="K13" t="s">
+        <v>3223</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>3545</v>
+      </c>
+      <c r="M13">
+        <v>651</v>
+      </c>
+      <c r="N13" t="s">
+        <v>3546</v>
+      </c>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4">
+        <v>43943</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>43936</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N6" r:id="rId1" xr:uid="{4C51F28C-A368-DA47-B5FB-CBDB0D3BB91F}"/>
-    <hyperlink ref="N7" r:id="rId2" xr:uid="{68F5DF97-42B3-5F45-892E-0093E19A8957}"/>
-    <hyperlink ref="N8" r:id="rId3" xr:uid="{3E5BD913-44B6-CE4A-975C-E93DB1C83B93}"/>
-    <hyperlink ref="N9" r:id="rId4" xr:uid="{F52A61F9-9CC3-0147-B1DC-1C716CBA9717}"/>
-    <hyperlink ref="N10" r:id="rId5" xr:uid="{60E03D8E-0712-4947-B7CE-877688E401DA}"/>
-    <hyperlink ref="N12" r:id="rId6" xr:uid="{1DAE6220-4728-6A47-B155-9BAC7EAA47A8}"/>
-    <hyperlink ref="N11" r:id="rId7" xr:uid="{9BFF6399-6446-B144-B29C-B0FD3595AC1F}"/>
+    <hyperlink ref="N6" r:id="rId1" xr:uid="{F28ACAE7-20DC-544F-A84D-371CF6FF5B26}"/>
+    <hyperlink ref="N7" r:id="rId2" xr:uid="{2CA47FC0-58A8-4842-8A94-403B3DB0E612}"/>
+    <hyperlink ref="N8" r:id="rId3" xr:uid="{2A5D76A7-212A-FF45-94CB-B9765B2AE80C}"/>
+    <hyperlink ref="N9" r:id="rId4" xr:uid="{99DB5D94-F8A7-9543-A23A-280A3D7FC7CB}"/>
+    <hyperlink ref="N10" r:id="rId5" xr:uid="{4D2C43C7-B49F-EA45-B50F-1177AD0417FF}"/>
+    <hyperlink ref="N12" r:id="rId6" xr:uid="{25096900-E45F-4E40-BF57-88A9E8056E23}"/>
+    <hyperlink ref="N11" r:id="rId7" xr:uid="{FD29AE63-4C14-F445-AC07-1286541A3CFC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -54540,10 +54611,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5218A77D-399C-1D47-B6D8-167C71D40314}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -54811,6 +54882,20 @@
       </c>
       <c r="E20" t="s">
         <v>3492</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>3222</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3541</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3542</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2765</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing dates, checking matching, running notebook through
</commit_message>
<xml_diff>
--- a/notebooks/manual_data.xlsx
+++ b/notebooks/manual_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholasdevito/Documents/GitHub/covid_trials_tracker-covid/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E8E8B3-503C-7C44-AB41-27F6C65E87FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB3C6B9-8C0B-7545-8857-306A8DEE74BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24520" windowHeight="14280" activeTab="5" xr2:uid="{EB2E916D-92E5-6547-902E-71CC9B785F8F}"/>
+    <workbookView xWindow="-32620" yWindow="5020" windowWidth="24520" windowHeight="14280" activeTab="2" xr2:uid="{EB2E916D-92E5-6547-902E-71CC9B785F8F}"/>
   </bookViews>
   <sheets>
     <sheet name="sponsor" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12305" uniqueCount="4815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12326" uniqueCount="4820">
   <si>
     <t>unique_spon_names</t>
   </si>
@@ -14530,6 +14530,22 @@
   </si>
   <si>
     <t>https://clinicaltrials.gov/ct2/show/NCT04350580</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1101/2020.04.20.20072470</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1101/2020.04.18.20071134</t>
+  </si>
+  <si>
+    <t>EUCTR2020-001553-48</t>
+  </si>
+  <si>
+    <t>Drug: cholecalciferol 200,000 IU
+Drug: cholecalciferol 50,000 IU</t>
+  </si>
+  <si>
+    <t>https://clinicaltrials.gov/ct2/show/NCT04344041</t>
   </si>
 </sst>
 </file>
@@ -22557,7 +22573,7 @@
   <dimension ref="A1:F1478"/>
   <sheetViews>
     <sheetView topLeftCell="A954" workbookViewId="0">
-      <selection activeCell="B960" sqref="B960"/>
+      <selection activeCell="A959" sqref="A959"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -49237,8 +49253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ABCEDD8-99CD-E64D-83C4-23A5F7177A3C}">
   <dimension ref="A1:C1987"/>
   <sheetViews>
-    <sheetView topLeftCell="A1448" workbookViewId="0">
-      <selection activeCell="E1455" sqref="E1455"/>
+    <sheetView tabSelected="1" topLeftCell="A1410" workbookViewId="0">
+      <selection activeCell="A1470" sqref="A1470"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -65452,7 +65468,15 @@
       </c>
     </row>
     <row r="1474" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1474" s="12"/>
+      <c r="A1474" s="12" t="s">
+        <v>957</v>
+      </c>
+      <c r="B1474" s="12" t="s">
+        <v>2202</v>
+      </c>
+      <c r="C1474" s="7">
+        <v>43900</v>
+      </c>
     </row>
     <row r="1475" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1475" s="12"/>
@@ -67003,8 +67027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F8C4E0-02D7-BD4E-9875-A292DA5969FB}">
   <dimension ref="A1:D997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -67505,17 +67529,33 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="5"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="5"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
+    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>3062</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>4815</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>2204</v>
+      </c>
+      <c r="D36" s="7">
+        <v>43945</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>2014</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>4816</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>2204</v>
+      </c>
+      <c r="D37" s="8">
+        <v>43944</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="5"/>
@@ -73310,6 +73350,8 @@
     <hyperlink ref="B34" r:id="rId31" xr:uid="{4FC47996-C7B4-1147-B9D8-F91D173C9B21}"/>
     <hyperlink ref="B35" r:id="rId32" xr:uid="{58943300-8E1B-0541-AC1F-AC3403293E76}"/>
     <hyperlink ref="B30" r:id="rId33" xr:uid="{9DA68BD0-0378-E945-B7FA-245F83886F30}"/>
+    <hyperlink ref="B36" r:id="rId34" xr:uid="{5425D789-73D7-DF45-9C0E-4F5E908B4E63}"/>
+    <hyperlink ref="B37" r:id="rId35" xr:uid="{83CD14A5-40B4-5F4B-99C7-98665DBD7138}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -73317,11 +73359,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2897C11-45D0-1143-9B66-314A64F11CA5}">
-  <dimension ref="A1:Q18"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -74244,6 +74286,53 @@
         <v>43943</v>
       </c>
     </row>
+    <row r="19" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>4807</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1796</v>
+      </c>
+      <c r="C19" s="4">
+        <v>43930</v>
+      </c>
+      <c r="D19" s="4">
+        <v>43936</v>
+      </c>
+      <c r="E19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>2341</v>
+      </c>
+      <c r="H19" t="s">
+        <v>1810</v>
+      </c>
+      <c r="I19" t="s">
+        <v>1799</v>
+      </c>
+      <c r="J19" t="s">
+        <v>1808</v>
+      </c>
+      <c r="K19" t="s">
+        <v>4808</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>4818</v>
+      </c>
+      <c r="M19">
+        <v>260</v>
+      </c>
+      <c r="N19" s="10" t="s">
+        <v>4819</v>
+      </c>
+      <c r="P19" s="4">
+        <v>43942</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>43943</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="N6" r:id="rId1" xr:uid="{F28ACAE7-20DC-544F-A84D-371CF6FF5B26}"/>
@@ -74258,6 +74347,7 @@
     <hyperlink ref="N16" r:id="rId10" xr:uid="{D6056C57-FAFE-D249-8D4B-75E83F2B2755}"/>
     <hyperlink ref="N17" r:id="rId11" xr:uid="{5DF8AAD2-E008-3845-8EBE-06760216E300}"/>
     <hyperlink ref="N18" r:id="rId12" xr:uid="{0267BC37-FB1D-7B44-ABA8-EB05EFFC0233}"/>
+    <hyperlink ref="N19" r:id="rId13" xr:uid="{B2F4FE5D-DDE5-4D43-831B-DD25C3EA315E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -74265,10 +74355,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5218A77D-399C-1D47-B6D8-167C71D40314}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -74708,6 +74798,20 @@
         <v>4154</v>
       </c>
       <c r="D33" t="s">
+        <v>2762</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>4802</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4817</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4155</v>
+      </c>
+      <c r="D34" t="s">
         <v>2762</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final Update with figures
</commit_message>
<xml_diff>
--- a/notebooks/manual_data.xlsx
+++ b/notebooks/manual_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholasdevito/Documents/GitHub/covid_trials_tracker-covid/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B261DD-190B-0B46-9AD5-A0CE1FB33BF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1CDAC5-F59C-4042-974E-C1B046DA711E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2360" yWindow="880" windowWidth="22220" windowHeight="14380" activeTab="4" xr2:uid="{EB2E916D-92E5-6547-902E-71CC9B785F8F}"/>
+    <workbookView xWindow="4200" yWindow="2020" windowWidth="22220" windowHeight="14380" activeTab="1" xr2:uid="{EB2E916D-92E5-6547-902E-71CC9B785F8F}"/>
   </bookViews>
   <sheets>
     <sheet name="sponsor" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12396" uniqueCount="4839">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12429" uniqueCount="4851">
   <si>
     <t>unique_spon_names</t>
   </si>
@@ -13643,9 +13643,6 @@
     <t>Sedation with sevoflurane versus propofol in patients with Acute Respiratory Distress Syndrome caused by COVID-19 infection</t>
   </si>
   <si>
-    <t>Preventative Drug Treatment for COVID-19 Infectious Disease</t>
-  </si>
-  <si>
     <t>Use of a respiratory multiplex PCR and procalcitonin to reduce antibiotic exposure in patients with severe confirmed COVID-19 pneumonia</t>
   </si>
   <si>
@@ -14607,6 +14604,47 @@
   </si>
   <si>
     <t>Sarilumab; azithromycin; hydroxychloroquine</t>
+  </si>
+  <si>
+    <t>RBR-9ktwx6</t>
+  </si>
+  <si>
+    <t>REBEC</t>
+  </si>
+  <si>
+    <t>Socidade Brasileira de Reumatologia</t>
+  </si>
+  <si>
+    <t>Evaluation of the effect of chronic use of Antimalarials on the frequency of infection with the New Corona Virus 2019 (Severe Acute Respiratory Syndrome Coronavirus 2 - SARS-CoV-2) in patients with Immunomedical Rheumatic Diseases</t>
+  </si>
+  <si>
+    <t>Chloroquine and Hydroxychloroquine</t>
+  </si>
+  <si>
+    <t>http://www.ensaiosclinicos.gov.br/rg/RBR-9ktwx6/</t>
+  </si>
+  <si>
+    <t>EUCTR2020-001224-33</t>
+  </si>
+  <si>
+    <t>NCT04352933</t>
+  </si>
+  <si>
+    <t>EUCTR2020-001331-26</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>PROLIFIC ChemoprophylaxisTrial (COVID-19)</t>
+  </si>
+  <si>
+    <t>Drug: Hydroxychloroquine - Daily dosing
+Drug: Hydroxychloroquine - Weekly Dosing
+Other: Matched Placebo Hydroxychloroquine</t>
+  </si>
+  <si>
+    <t>https://clinicaltrials.gov/ct2/show/NCT04352933</t>
   </si>
 </sst>
 </file>
@@ -15063,10 +15101,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D462C6-375D-2A4D-81F0-358CC20C32FE}">
-  <dimension ref="A1:B946"/>
+  <dimension ref="A1:B947"/>
   <sheetViews>
-    <sheetView topLeftCell="A864" workbookViewId="0">
-      <selection activeCell="A880" sqref="A880"/>
+    <sheetView topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15445,7 +15483,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>4822</v>
+        <v>4821</v>
       </c>
       <c r="B47" t="s">
         <v>2236</v>
@@ -16013,10 +16051,10 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>4804</v>
+        <v>4803</v>
       </c>
       <c r="B118" t="s">
-        <v>4804</v>
+        <v>4803</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
@@ -22641,6 +22679,14 @@
       </c>
       <c r="B946" t="s">
         <v>414</v>
+      </c>
+    </row>
+    <row r="947" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A947" t="s">
+        <v>4840</v>
+      </c>
+      <c r="B947" t="s">
+        <v>4840</v>
       </c>
     </row>
   </sheetData>
@@ -22655,10 +22701,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC06582-2DEF-3F4C-9BDF-F5E9FA92249B}">
-  <dimension ref="A1:F1480"/>
+  <dimension ref="A1:F1481"/>
   <sheetViews>
-    <sheetView topLeftCell="A748" workbookViewId="0">
-      <selection activeCell="C759" sqref="C759"/>
+    <sheetView tabSelected="1" topLeftCell="A1470" workbookViewId="0">
+      <selection activeCell="B1481" sqref="B1481"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24631,7 +24677,7 @@
         <v>1055</v>
       </c>
       <c r="E109" s="27" t="s">
-        <v>4646</v>
+        <v>4645</v>
       </c>
       <c r="F109" s="26"/>
     </row>
@@ -24700,10 +24746,10 @@
         <v>1049</v>
       </c>
       <c r="D113" s="27" t="s">
+        <v>4661</v>
+      </c>
+      <c r="E113" s="27" t="s">
         <v>4662</v>
-      </c>
-      <c r="E113" s="27" t="s">
-        <v>4663</v>
       </c>
       <c r="F113" s="26"/>
     </row>
@@ -24808,10 +24854,10 @@
         <v>1049</v>
       </c>
       <c r="D119" s="25" t="s">
-        <v>4766</v>
+        <v>4765</v>
       </c>
       <c r="E119" s="27" t="s">
-        <v>4694</v>
+        <v>4693</v>
       </c>
       <c r="F119" s="26"/>
     </row>
@@ -24892,7 +24938,7 @@
         <v>4126</v>
       </c>
       <c r="B124" s="26" t="s">
-        <v>4774</v>
+        <v>4773</v>
       </c>
       <c r="C124" s="27" t="s">
         <v>1049</v>
@@ -24946,7 +24992,7 @@
         <v>4163</v>
       </c>
       <c r="B127" s="26" t="s">
-        <v>4527</v>
+        <v>4526</v>
       </c>
       <c r="C127" s="27" t="s">
         <v>1049</v>
@@ -24964,7 +25010,7 @@
         <v>4220</v>
       </c>
       <c r="B128" s="26" t="s">
-        <v>4583</v>
+        <v>4582</v>
       </c>
       <c r="C128" s="27" t="s">
         <v>1049</v>
@@ -29324,7 +29370,7 @@
         <v>4174</v>
       </c>
       <c r="B367" s="26" t="s">
-        <v>4538</v>
+        <v>4537</v>
       </c>
       <c r="C367" s="27" t="s">
         <v>1756</v>
@@ -29342,7 +29388,7 @@
         <v>4175</v>
       </c>
       <c r="B368" s="26" t="s">
-        <v>4539</v>
+        <v>4538</v>
       </c>
       <c r="C368" s="27" t="s">
         <v>1756</v>
@@ -29360,7 +29406,7 @@
         <v>4179</v>
       </c>
       <c r="B369" s="26" t="s">
-        <v>4543</v>
+        <v>4542</v>
       </c>
       <c r="C369" s="27" t="s">
         <v>1756</v>
@@ -29378,7 +29424,7 @@
         <v>4182</v>
       </c>
       <c r="B370" s="26" t="s">
-        <v>4546</v>
+        <v>4545</v>
       </c>
       <c r="C370" s="27" t="s">
         <v>1756</v>
@@ -29396,7 +29442,7 @@
         <v>4183</v>
       </c>
       <c r="B371" s="26" t="s">
-        <v>4547</v>
+        <v>4546</v>
       </c>
       <c r="C371" s="27" t="s">
         <v>1756</v>
@@ -29414,7 +29460,7 @@
         <v>4184</v>
       </c>
       <c r="B372" s="26" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
       <c r="C372" s="27" t="s">
         <v>1756</v>
@@ -29432,7 +29478,7 @@
         <v>4185</v>
       </c>
       <c r="B373" s="26" t="s">
-        <v>4549</v>
+        <v>4548</v>
       </c>
       <c r="C373" s="27" t="s">
         <v>1756</v>
@@ -29450,7 +29496,7 @@
         <v>4190</v>
       </c>
       <c r="B374" s="26" t="s">
-        <v>4781</v>
+        <v>4780</v>
       </c>
       <c r="C374" s="27" t="s">
         <v>1756</v>
@@ -29468,7 +29514,7 @@
         <v>4194</v>
       </c>
       <c r="B375" s="26" t="s">
-        <v>4557</v>
+        <v>4556</v>
       </c>
       <c r="C375" s="27" t="s">
         <v>1756</v>
@@ -29486,7 +29532,7 @@
         <v>4195</v>
       </c>
       <c r="B376" s="26" t="s">
-        <v>4558</v>
+        <v>4557</v>
       </c>
       <c r="C376" s="27" t="s">
         <v>1756</v>
@@ -29504,7 +29550,7 @@
         <v>4203</v>
       </c>
       <c r="B377" s="26" t="s">
-        <v>4566</v>
+        <v>4565</v>
       </c>
       <c r="C377" s="27" t="s">
         <v>1756</v>
@@ -29522,7 +29568,7 @@
         <v>4204</v>
       </c>
       <c r="B378" s="26" t="s">
-        <v>4567</v>
+        <v>4566</v>
       </c>
       <c r="C378" s="27" t="s">
         <v>1756</v>
@@ -29540,7 +29586,7 @@
         <v>4207</v>
       </c>
       <c r="B379" s="26" t="s">
-        <v>4570</v>
+        <v>4569</v>
       </c>
       <c r="C379" s="27" t="s">
         <v>1756</v>
@@ -29558,7 +29604,7 @@
         <v>4209</v>
       </c>
       <c r="B380" s="26" t="s">
-        <v>4572</v>
+        <v>4571</v>
       </c>
       <c r="C380" s="27" t="s">
         <v>1756</v>
@@ -29576,7 +29622,7 @@
         <v>4213</v>
       </c>
       <c r="B381" s="26" t="s">
-        <v>4576</v>
+        <v>4575</v>
       </c>
       <c r="C381" s="27" t="s">
         <v>1756</v>
@@ -29594,7 +29640,7 @@
         <v>4216</v>
       </c>
       <c r="B382" s="26" t="s">
-        <v>4579</v>
+        <v>4578</v>
       </c>
       <c r="C382" s="27" t="s">
         <v>1756</v>
@@ -29992,7 +30038,7 @@
         <v>4170</v>
       </c>
       <c r="B404" s="26" t="s">
-        <v>4534</v>
+        <v>4533</v>
       </c>
       <c r="C404" s="27" t="s">
         <v>3445</v>
@@ -30010,7 +30056,7 @@
         <v>4173</v>
       </c>
       <c r="B405" s="26" t="s">
-        <v>4537</v>
+        <v>4536</v>
       </c>
       <c r="C405" s="27" t="s">
         <v>3445</v>
@@ -30028,7 +30074,7 @@
         <v>4187</v>
       </c>
       <c r="B406" s="26" t="s">
-        <v>4551</v>
+        <v>4550</v>
       </c>
       <c r="C406" s="27" t="s">
         <v>3445</v>
@@ -30046,7 +30092,7 @@
         <v>4189</v>
       </c>
       <c r="B407" s="26" t="s">
-        <v>4553</v>
+        <v>4552</v>
       </c>
       <c r="C407" s="27" t="s">
         <v>3445</v>
@@ -30064,7 +30110,7 @@
         <v>4206</v>
       </c>
       <c r="B408" s="26" t="s">
-        <v>4569</v>
+        <v>4568</v>
       </c>
       <c r="C408" s="27" t="s">
         <v>3445</v>
@@ -30082,7 +30128,7 @@
         <v>4210</v>
       </c>
       <c r="B409" s="26" t="s">
-        <v>4573</v>
+        <v>4572</v>
       </c>
       <c r="C409" s="27" t="s">
         <v>3445</v>
@@ -31318,7 +31364,7 @@
         <v>4168</v>
       </c>
       <c r="B477" s="26" t="s">
-        <v>4532</v>
+        <v>4531</v>
       </c>
       <c r="C477" s="25" t="s">
         <v>3443</v>
@@ -31336,7 +31382,7 @@
         <v>4180</v>
       </c>
       <c r="B478" s="26" t="s">
-        <v>4544</v>
+        <v>4543</v>
       </c>
       <c r="C478" s="27" t="s">
         <v>3443</v>
@@ -31354,7 +31400,7 @@
         <v>4192</v>
       </c>
       <c r="B479" s="26" t="s">
-        <v>4555</v>
+        <v>4554</v>
       </c>
       <c r="C479" s="27" t="s">
         <v>3443</v>
@@ -31372,7 +31418,7 @@
         <v>4215</v>
       </c>
       <c r="B480" s="26" t="s">
-        <v>4578</v>
+        <v>4577</v>
       </c>
       <c r="C480" s="25" t="s">
         <v>3443</v>
@@ -35320,10 +35366,10 @@
         <v>1057</v>
       </c>
       <c r="D699" s="18" t="s">
+        <v>4814</v>
+      </c>
+      <c r="E699" s="18" t="s">
         <v>4815</v>
-      </c>
-      <c r="E699" s="18" t="s">
-        <v>4816</v>
       </c>
       <c r="F699" s="26"/>
     </row>
@@ -36400,10 +36446,10 @@
         <v>1057</v>
       </c>
       <c r="D759" s="18" t="s">
+        <v>4836</v>
+      </c>
+      <c r="E759" s="18" t="s">
         <v>4837</v>
-      </c>
-      <c r="E759" s="18" t="s">
-        <v>4838</v>
       </c>
       <c r="F759" s="26"/>
     </row>
@@ -36940,10 +36986,10 @@
         <v>1057</v>
       </c>
       <c r="D789" s="18" t="s">
+        <v>4828</v>
+      </c>
+      <c r="E789" s="18" t="s">
         <v>4829</v>
-      </c>
-      <c r="E789" s="18" t="s">
-        <v>4830</v>
       </c>
       <c r="F789" s="26"/>
     </row>
@@ -37606,10 +37652,10 @@
         <v>1057</v>
       </c>
       <c r="D826" s="26" t="s">
+        <v>4593</v>
+      </c>
+      <c r="E826" s="26" t="s">
         <v>4594</v>
-      </c>
-      <c r="E826" s="26" t="s">
-        <v>4595</v>
       </c>
       <c r="F826" s="26"/>
     </row>
@@ -37624,7 +37670,7 @@
         <v>1057</v>
       </c>
       <c r="D827" s="26" t="s">
-        <v>4745</v>
+        <v>4744</v>
       </c>
       <c r="E827" s="26" t="s">
         <v>2713</v>
@@ -37642,10 +37688,10 @@
         <v>1057</v>
       </c>
       <c r="D828" s="18" t="s">
-        <v>4596</v>
+        <v>4595</v>
       </c>
       <c r="E828" s="18" t="s">
-        <v>4596</v>
+        <v>4595</v>
       </c>
       <c r="F828" s="26"/>
     </row>
@@ -37678,7 +37724,7 @@
         <v>1057</v>
       </c>
       <c r="D830" s="26" t="s">
-        <v>4597</v>
+        <v>4596</v>
       </c>
       <c r="E830" s="26" t="s">
         <v>1916</v>
@@ -37714,10 +37760,10 @@
         <v>1057</v>
       </c>
       <c r="D832" s="22" t="s">
+        <v>4598</v>
+      </c>
+      <c r="E832" s="22" t="s">
         <v>4599</v>
-      </c>
-      <c r="E832" s="22" t="s">
-        <v>4600</v>
       </c>
       <c r="F832" s="26"/>
     </row>
@@ -37732,10 +37778,10 @@
         <v>1057</v>
       </c>
       <c r="D833" s="26" t="s">
-        <v>4746</v>
+        <v>4745</v>
       </c>
       <c r="E833" s="26" t="s">
-        <v>4601</v>
+        <v>4600</v>
       </c>
       <c r="F833" s="26"/>
     </row>
@@ -37786,10 +37832,10 @@
         <v>1057</v>
       </c>
       <c r="D836" s="26" t="s">
-        <v>4747</v>
+        <v>4746</v>
       </c>
       <c r="E836" s="26" t="s">
-        <v>4602</v>
+        <v>4601</v>
       </c>
       <c r="F836" s="26"/>
     </row>
@@ -37822,10 +37868,10 @@
         <v>1057</v>
       </c>
       <c r="D838" s="26" t="s">
-        <v>4603</v>
+        <v>4602</v>
       </c>
       <c r="E838" s="26" t="s">
-        <v>4603</v>
+        <v>4602</v>
       </c>
       <c r="F838" s="26"/>
     </row>
@@ -37840,10 +37886,10 @@
         <v>1057</v>
       </c>
       <c r="D839" s="29" t="s">
-        <v>4604</v>
+        <v>4603</v>
       </c>
       <c r="E839" s="29" t="s">
-        <v>4604</v>
+        <v>4603</v>
       </c>
       <c r="F839" s="26"/>
     </row>
@@ -37858,10 +37904,10 @@
         <v>1057</v>
       </c>
       <c r="D840" s="27" t="s">
+        <v>4604</v>
+      </c>
+      <c r="E840" s="27" t="s">
         <v>4605</v>
-      </c>
-      <c r="E840" s="27" t="s">
-        <v>4606</v>
       </c>
       <c r="F840" s="26"/>
     </row>
@@ -37876,10 +37922,10 @@
         <v>1057</v>
       </c>
       <c r="D841" s="27" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="E841" s="29" t="s">
-        <v>4607</v>
+        <v>4606</v>
       </c>
       <c r="F841" s="26"/>
     </row>
@@ -37894,10 +37940,10 @@
         <v>1057</v>
       </c>
       <c r="D842" s="26" t="s">
-        <v>4608</v>
+        <v>4607</v>
       </c>
       <c r="E842" s="26" t="s">
-        <v>4608</v>
+        <v>4607</v>
       </c>
       <c r="F842" s="26"/>
     </row>
@@ -37948,10 +37994,10 @@
         <v>1057</v>
       </c>
       <c r="D845" s="27" t="s">
+        <v>4608</v>
+      </c>
+      <c r="E845" s="27" t="s">
         <v>4609</v>
-      </c>
-      <c r="E845" s="27" t="s">
-        <v>4610</v>
       </c>
       <c r="F845" s="26"/>
     </row>
@@ -38002,10 +38048,10 @@
         <v>1057</v>
       </c>
       <c r="D848" s="26" t="s">
-        <v>4611</v>
+        <v>4610</v>
       </c>
       <c r="E848" s="26" t="s">
-        <v>4611</v>
+        <v>4610</v>
       </c>
       <c r="F848" s="26"/>
     </row>
@@ -38020,10 +38066,10 @@
         <v>1057</v>
       </c>
       <c r="D849" s="26" t="s">
+        <v>4611</v>
+      </c>
+      <c r="E849" s="26" t="s">
         <v>4612</v>
-      </c>
-      <c r="E849" s="26" t="s">
-        <v>4613</v>
       </c>
       <c r="F849" s="26"/>
     </row>
@@ -38038,10 +38084,10 @@
         <v>1057</v>
       </c>
       <c r="D850" s="26" t="s">
-        <v>4614</v>
+        <v>4613</v>
       </c>
       <c r="E850" s="26" t="s">
-        <v>4614</v>
+        <v>4613</v>
       </c>
       <c r="F850" s="26"/>
     </row>
@@ -38056,10 +38102,10 @@
         <v>1057</v>
       </c>
       <c r="D851" s="26" t="s">
-        <v>4615</v>
+        <v>4614</v>
       </c>
       <c r="E851" s="26" t="s">
-        <v>4615</v>
+        <v>4614</v>
       </c>
       <c r="F851" s="26"/>
     </row>
@@ -38074,10 +38120,10 @@
         <v>1057</v>
       </c>
       <c r="D852" s="26" t="s">
+        <v>4752</v>
+      </c>
+      <c r="E852" s="26" t="s">
         <v>4753</v>
-      </c>
-      <c r="E852" s="26" t="s">
-        <v>4754</v>
       </c>
       <c r="F852" s="26"/>
     </row>
@@ -38092,10 +38138,10 @@
         <v>1057</v>
       </c>
       <c r="D853" s="26" t="s">
-        <v>4616</v>
+        <v>4615</v>
       </c>
       <c r="E853" s="26" t="s">
-        <v>4616</v>
+        <v>4615</v>
       </c>
       <c r="F853" s="26"/>
     </row>
@@ -38146,10 +38192,10 @@
         <v>1057</v>
       </c>
       <c r="D856" s="26" t="s">
-        <v>4617</v>
+        <v>4616</v>
       </c>
       <c r="E856" s="26" t="s">
-        <v>4617</v>
+        <v>4616</v>
       </c>
       <c r="F856" s="26"/>
     </row>
@@ -38182,10 +38228,10 @@
         <v>1057</v>
       </c>
       <c r="D858" s="26" t="s">
+        <v>4617</v>
+      </c>
+      <c r="E858" s="26" t="s">
         <v>4618</v>
-      </c>
-      <c r="E858" s="26" t="s">
-        <v>4619</v>
       </c>
       <c r="F858" s="26"/>
     </row>
@@ -38218,10 +38264,10 @@
         <v>1057</v>
       </c>
       <c r="D860" s="26" t="s">
+        <v>4619</v>
+      </c>
+      <c r="E860" s="26" t="s">
         <v>4620</v>
-      </c>
-      <c r="E860" s="26" t="s">
-        <v>4621</v>
       </c>
       <c r="F860" s="26"/>
     </row>
@@ -38236,10 +38282,10 @@
         <v>1057</v>
       </c>
       <c r="D861" s="26" t="s">
+        <v>4621</v>
+      </c>
+      <c r="E861" s="26" t="s">
         <v>4622</v>
-      </c>
-      <c r="E861" s="26" t="s">
-        <v>4623</v>
       </c>
       <c r="F861" s="26"/>
     </row>
@@ -38254,10 +38300,10 @@
         <v>1057</v>
       </c>
       <c r="D862" s="26" t="s">
-        <v>4625</v>
+        <v>4624</v>
       </c>
       <c r="E862" s="26" t="s">
-        <v>4625</v>
+        <v>4624</v>
       </c>
       <c r="F862" s="26"/>
     </row>
@@ -38290,10 +38336,10 @@
         <v>1057</v>
       </c>
       <c r="D864" s="26" t="s">
-        <v>4626</v>
+        <v>4625</v>
       </c>
       <c r="E864" s="26" t="s">
-        <v>4626</v>
+        <v>4625</v>
       </c>
       <c r="F864" s="26"/>
     </row>
@@ -38308,10 +38354,10 @@
         <v>1057</v>
       </c>
       <c r="D865" s="26" t="s">
-        <v>4627</v>
+        <v>4626</v>
       </c>
       <c r="E865" s="26" t="s">
-        <v>4627</v>
+        <v>4626</v>
       </c>
       <c r="F865" s="26"/>
     </row>
@@ -38344,10 +38390,10 @@
         <v>1057</v>
       </c>
       <c r="D867" s="26" t="s">
+        <v>4627</v>
+      </c>
+      <c r="E867" s="26" t="s">
         <v>4628</v>
-      </c>
-      <c r="E867" s="26" t="s">
-        <v>4629</v>
       </c>
       <c r="F867" s="26"/>
     </row>
@@ -38380,10 +38426,10 @@
         <v>1057</v>
       </c>
       <c r="D869" s="26" t="s">
-        <v>4630</v>
+        <v>4629</v>
       </c>
       <c r="E869" s="29" t="s">
-        <v>4630</v>
+        <v>4629</v>
       </c>
       <c r="F869" s="26"/>
     </row>
@@ -38416,10 +38462,10 @@
         <v>1057</v>
       </c>
       <c r="D871" s="26" t="s">
-        <v>4632</v>
+        <v>4631</v>
       </c>
       <c r="E871" s="26" t="s">
-        <v>4632</v>
+        <v>4631</v>
       </c>
       <c r="F871" s="26"/>
     </row>
@@ -38434,10 +38480,10 @@
         <v>1057</v>
       </c>
       <c r="D872" s="26" t="s">
-        <v>4633</v>
+        <v>4632</v>
       </c>
       <c r="E872" s="26" t="s">
-        <v>4633</v>
+        <v>4632</v>
       </c>
       <c r="F872" s="26"/>
     </row>
@@ -38452,10 +38498,10 @@
         <v>1057</v>
       </c>
       <c r="D873" s="27" t="s">
-        <v>4756</v>
+        <v>4755</v>
       </c>
       <c r="E873" s="26" t="s">
-        <v>4634</v>
+        <v>4633</v>
       </c>
       <c r="F873" s="26"/>
     </row>
@@ -38470,10 +38516,10 @@
         <v>1057</v>
       </c>
       <c r="D874" s="26" t="s">
-        <v>4635</v>
+        <v>4634</v>
       </c>
       <c r="E874" s="26" t="s">
-        <v>4635</v>
+        <v>4634</v>
       </c>
       <c r="F874" s="26"/>
     </row>
@@ -38488,10 +38534,10 @@
         <v>1057</v>
       </c>
       <c r="D875" s="26" t="s">
+        <v>4635</v>
+      </c>
+      <c r="E875" s="26" t="s">
         <v>4636</v>
-      </c>
-      <c r="E875" s="26" t="s">
-        <v>4637</v>
       </c>
       <c r="F875" s="26"/>
     </row>
@@ -38506,10 +38552,10 @@
         <v>1057</v>
       </c>
       <c r="D876" s="26" t="s">
-        <v>4638</v>
+        <v>4637</v>
       </c>
       <c r="E876" s="26" t="s">
-        <v>4638</v>
+        <v>4637</v>
       </c>
       <c r="F876" s="26"/>
     </row>
@@ -38542,10 +38588,10 @@
         <v>1057</v>
       </c>
       <c r="D878" s="26" t="s">
-        <v>4639</v>
+        <v>4638</v>
       </c>
       <c r="E878" s="26" t="s">
-        <v>4639</v>
+        <v>4638</v>
       </c>
       <c r="F878" s="26"/>
     </row>
@@ -38560,10 +38606,10 @@
         <v>1057</v>
       </c>
       <c r="D879" s="27" t="s">
+        <v>4639</v>
+      </c>
+      <c r="E879" s="27" t="s">
         <v>4640</v>
-      </c>
-      <c r="E879" s="27" t="s">
-        <v>4641</v>
       </c>
       <c r="F879" s="26"/>
     </row>
@@ -38578,10 +38624,10 @@
         <v>1057</v>
       </c>
       <c r="D880" s="27" t="s">
+        <v>4641</v>
+      </c>
+      <c r="E880" s="27" t="s">
         <v>4642</v>
-      </c>
-      <c r="E880" s="27" t="s">
-        <v>4643</v>
       </c>
       <c r="F880" s="26"/>
     </row>
@@ -38596,10 +38642,10 @@
         <v>1057</v>
       </c>
       <c r="D881" s="27" t="s">
-        <v>4644</v>
+        <v>4643</v>
       </c>
       <c r="E881" s="27" t="s">
-        <v>4644</v>
+        <v>4643</v>
       </c>
       <c r="F881" s="26"/>
     </row>
@@ -38614,7 +38660,7 @@
         <v>1057</v>
       </c>
       <c r="D882" s="27" t="s">
-        <v>4645</v>
+        <v>4644</v>
       </c>
       <c r="E882" s="27" t="s">
         <v>1934</v>
@@ -38668,10 +38714,10 @@
         <v>1057</v>
       </c>
       <c r="D885" s="27" t="s">
+        <v>4646</v>
+      </c>
+      <c r="E885" s="27" t="s">
         <v>4647</v>
-      </c>
-      <c r="E885" s="27" t="s">
-        <v>4648</v>
       </c>
       <c r="F885" s="26"/>
     </row>
@@ -38686,7 +38732,7 @@
         <v>1057</v>
       </c>
       <c r="D886" s="27" t="s">
-        <v>4649</v>
+        <v>4648</v>
       </c>
       <c r="E886" s="27" t="s">
         <v>3426</v>
@@ -38704,10 +38750,10 @@
         <v>1057</v>
       </c>
       <c r="D887" s="27" t="s">
+        <v>4649</v>
+      </c>
+      <c r="E887" s="27" t="s">
         <v>4650</v>
-      </c>
-      <c r="E887" s="27" t="s">
-        <v>4651</v>
       </c>
       <c r="F887" s="26"/>
     </row>
@@ -38722,7 +38768,7 @@
         <v>1057</v>
       </c>
       <c r="D888" s="27" t="s">
-        <v>4636</v>
+        <v>4635</v>
       </c>
       <c r="E888" s="27" t="s">
         <v>2713</v>
@@ -38776,10 +38822,10 @@
         <v>1057</v>
       </c>
       <c r="D891" s="27" t="s">
-        <v>4615</v>
+        <v>4614</v>
       </c>
       <c r="E891" s="27" t="s">
-        <v>4615</v>
+        <v>4614</v>
       </c>
       <c r="F891" s="26"/>
     </row>
@@ -38812,10 +38858,10 @@
         <v>1057</v>
       </c>
       <c r="D893" s="27" t="s">
-        <v>4655</v>
+        <v>4654</v>
       </c>
       <c r="E893" s="27" t="s">
-        <v>4655</v>
+        <v>4654</v>
       </c>
       <c r="F893" s="26"/>
     </row>
@@ -38848,7 +38894,7 @@
         <v>1057</v>
       </c>
       <c r="D895" s="27" t="s">
-        <v>4636</v>
+        <v>4635</v>
       </c>
       <c r="E895" s="27" t="s">
         <v>2713</v>
@@ -38866,10 +38912,10 @@
         <v>1057</v>
       </c>
       <c r="D896" s="27" t="s">
+        <v>4655</v>
+      </c>
+      <c r="E896" s="27" t="s">
         <v>4656</v>
-      </c>
-      <c r="E896" s="27" t="s">
-        <v>4657</v>
       </c>
       <c r="F896" s="26"/>
     </row>
@@ -38884,10 +38930,10 @@
         <v>1057</v>
       </c>
       <c r="D897" s="26" t="s">
+        <v>4657</v>
+      </c>
+      <c r="E897" s="26" t="s">
         <v>4658</v>
-      </c>
-      <c r="E897" s="26" t="s">
-        <v>4659</v>
       </c>
       <c r="F897" s="26"/>
     </row>
@@ -38920,10 +38966,10 @@
         <v>1057</v>
       </c>
       <c r="D899" s="27" t="s">
-        <v>4660</v>
+        <v>4659</v>
       </c>
       <c r="E899" s="27" t="s">
-        <v>4660</v>
+        <v>4659</v>
       </c>
       <c r="F899" s="26"/>
     </row>
@@ -38974,10 +39020,10 @@
         <v>1057</v>
       </c>
       <c r="D902" s="27" t="s">
-        <v>4758</v>
+        <v>4757</v>
       </c>
       <c r="E902" s="27" t="s">
-        <v>4661</v>
+        <v>4660</v>
       </c>
       <c r="F902" s="26"/>
     </row>
@@ -38992,10 +39038,10 @@
         <v>1057</v>
       </c>
       <c r="D903" s="27" t="s">
+        <v>4663</v>
+      </c>
+      <c r="E903" s="27" t="s">
         <v>4664</v>
-      </c>
-      <c r="E903" s="27" t="s">
-        <v>4665</v>
       </c>
       <c r="F903" s="26"/>
     </row>
@@ -39010,10 +39056,10 @@
         <v>1057</v>
       </c>
       <c r="D904" s="27" t="s">
+        <v>4665</v>
+      </c>
+      <c r="E904" s="27" t="s">
         <v>4666</v>
-      </c>
-      <c r="E904" s="27" t="s">
-        <v>4667</v>
       </c>
       <c r="F904" s="26"/>
     </row>
@@ -39028,10 +39074,10 @@
         <v>1057</v>
       </c>
       <c r="D905" s="27" t="s">
+        <v>4667</v>
+      </c>
+      <c r="E905" s="27" t="s">
         <v>4668</v>
-      </c>
-      <c r="E905" s="27" t="s">
-        <v>4669</v>
       </c>
       <c r="F905" s="26"/>
     </row>
@@ -39040,7 +39086,7 @@
         <v>4048</v>
       </c>
       <c r="B906" s="26" t="s">
-        <v>4759</v>
+        <v>4758</v>
       </c>
       <c r="C906" s="27" t="s">
         <v>1057</v>
@@ -39082,10 +39128,10 @@
         <v>1057</v>
       </c>
       <c r="D908" s="27" t="s">
+        <v>4669</v>
+      </c>
+      <c r="E908" s="27" t="s">
         <v>4670</v>
-      </c>
-      <c r="E908" s="27" t="s">
-        <v>4671</v>
       </c>
       <c r="F908" s="26"/>
     </row>
@@ -39118,10 +39164,10 @@
         <v>1057</v>
       </c>
       <c r="D910" s="27" t="s">
+        <v>4671</v>
+      </c>
+      <c r="E910" s="27" t="s">
         <v>4672</v>
-      </c>
-      <c r="E910" s="27" t="s">
-        <v>4673</v>
       </c>
       <c r="F910" s="26"/>
     </row>
@@ -39136,10 +39182,10 @@
         <v>1057</v>
       </c>
       <c r="D911" s="27" t="s">
-        <v>4674</v>
+        <v>4673</v>
       </c>
       <c r="E911" s="27" t="s">
-        <v>4674</v>
+        <v>4673</v>
       </c>
       <c r="F911" s="26"/>
     </row>
@@ -39148,16 +39194,16 @@
         <v>4063</v>
       </c>
       <c r="B912" s="26" t="s">
-        <v>4760</v>
+        <v>4759</v>
       </c>
       <c r="C912" s="27" t="s">
         <v>1057</v>
       </c>
       <c r="D912" s="27" t="s">
-        <v>4674</v>
+        <v>4673</v>
       </c>
       <c r="E912" s="27" t="s">
-        <v>4674</v>
+        <v>4673</v>
       </c>
       <c r="F912" s="26"/>
     </row>
@@ -39172,10 +39218,10 @@
         <v>1057</v>
       </c>
       <c r="D913" s="27" t="s">
-        <v>4675</v>
+        <v>4674</v>
       </c>
       <c r="E913" s="27" t="s">
-        <v>4675</v>
+        <v>4674</v>
       </c>
       <c r="F913" s="26"/>
     </row>
@@ -39184,16 +39230,16 @@
         <v>4068</v>
       </c>
       <c r="B914" s="26" t="s">
-        <v>4761</v>
+        <v>4760</v>
       </c>
       <c r="C914" s="27" t="s">
         <v>1057</v>
       </c>
       <c r="D914" s="27" t="s">
+        <v>4675</v>
+      </c>
+      <c r="E914" s="27" t="s">
         <v>4676</v>
-      </c>
-      <c r="E914" s="27" t="s">
-        <v>4677</v>
       </c>
       <c r="F914" s="26"/>
     </row>
@@ -39208,10 +39254,10 @@
         <v>1057</v>
       </c>
       <c r="D915" s="27" t="s">
-        <v>4762</v>
+        <v>4761</v>
       </c>
       <c r="E915" s="27" t="s">
-        <v>4678</v>
+        <v>4677</v>
       </c>
       <c r="F915" s="26"/>
     </row>
@@ -39226,10 +39272,10 @@
         <v>1057</v>
       </c>
       <c r="D916" s="27" t="s">
-        <v>4763</v>
+        <v>4762</v>
       </c>
       <c r="E916" s="27" t="s">
-        <v>4679</v>
+        <v>4678</v>
       </c>
       <c r="F916" s="26"/>
     </row>
@@ -39244,10 +39290,10 @@
         <v>1057</v>
       </c>
       <c r="D917" s="27" t="s">
+        <v>4679</v>
+      </c>
+      <c r="E917" s="27" t="s">
         <v>4680</v>
-      </c>
-      <c r="E917" s="27" t="s">
-        <v>4681</v>
       </c>
       <c r="F917" s="26"/>
     </row>
@@ -39256,16 +39302,16 @@
         <v>4072</v>
       </c>
       <c r="B918" s="26" t="s">
-        <v>4764</v>
+        <v>4763</v>
       </c>
       <c r="C918" s="27" t="s">
         <v>1057</v>
       </c>
       <c r="D918" s="27" t="s">
+        <v>4681</v>
+      </c>
+      <c r="E918" s="27" t="s">
         <v>4682</v>
-      </c>
-      <c r="E918" s="27" t="s">
-        <v>4683</v>
       </c>
       <c r="F918" s="26"/>
     </row>
@@ -39280,10 +39326,10 @@
         <v>1057</v>
       </c>
       <c r="D919" s="27" t="s">
-        <v>4684</v>
+        <v>4683</v>
       </c>
       <c r="E919" s="27" t="s">
-        <v>4684</v>
+        <v>4683</v>
       </c>
       <c r="F919" s="26"/>
     </row>
@@ -39298,10 +39344,10 @@
         <v>1057</v>
       </c>
       <c r="D920" s="27" t="s">
-        <v>4765</v>
+        <v>4764</v>
       </c>
       <c r="E920" s="27" t="s">
-        <v>4685</v>
+        <v>4684</v>
       </c>
       <c r="F920" s="26"/>
     </row>
@@ -39316,10 +39362,10 @@
         <v>1057</v>
       </c>
       <c r="D921" s="27" t="s">
-        <v>4625</v>
+        <v>4624</v>
       </c>
       <c r="E921" s="27" t="s">
-        <v>4625</v>
+        <v>4624</v>
       </c>
       <c r="F921" s="26"/>
     </row>
@@ -39334,10 +39380,10 @@
         <v>1057</v>
       </c>
       <c r="D922" s="27" t="s">
+        <v>4685</v>
+      </c>
+      <c r="E922" s="27" t="s">
         <v>4686</v>
-      </c>
-      <c r="E922" s="27" t="s">
-        <v>4687</v>
       </c>
       <c r="F922" s="26"/>
     </row>
@@ -39352,10 +39398,10 @@
         <v>1057</v>
       </c>
       <c r="D923" s="27" t="s">
+        <v>4687</v>
+      </c>
+      <c r="E923" s="27" t="s">
         <v>4688</v>
-      </c>
-      <c r="E923" s="27" t="s">
-        <v>4689</v>
       </c>
       <c r="F923" s="26"/>
     </row>
@@ -39370,10 +39416,10 @@
         <v>1057</v>
       </c>
       <c r="D924" s="27" t="s">
+        <v>4689</v>
+      </c>
+      <c r="E924" s="27" t="s">
         <v>4690</v>
-      </c>
-      <c r="E924" s="27" t="s">
-        <v>4691</v>
       </c>
       <c r="F924" s="26"/>
     </row>
@@ -39388,10 +39434,10 @@
         <v>1057</v>
       </c>
       <c r="D925" s="27" t="s">
-        <v>4693</v>
+        <v>4692</v>
       </c>
       <c r="E925" s="27" t="s">
-        <v>4693</v>
+        <v>4692</v>
       </c>
       <c r="F925" s="26"/>
     </row>
@@ -39442,10 +39488,10 @@
         <v>1057</v>
       </c>
       <c r="D928" s="27" t="s">
-        <v>4767</v>
+        <v>4766</v>
       </c>
       <c r="E928" s="27" t="s">
-        <v>4695</v>
+        <v>4694</v>
       </c>
       <c r="F928" s="26"/>
     </row>
@@ -39460,10 +39506,10 @@
         <v>1057</v>
       </c>
       <c r="D929" s="27" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
       <c r="E929" s="27" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
       <c r="F929" s="26"/>
     </row>
@@ -39532,10 +39578,10 @@
         <v>1057</v>
       </c>
       <c r="D933" s="27" t="s">
-        <v>4768</v>
+        <v>4767</v>
       </c>
       <c r="E933" s="27" t="s">
-        <v>4697</v>
+        <v>4696</v>
       </c>
       <c r="F933" s="26"/>
     </row>
@@ -39550,10 +39596,10 @@
         <v>1057</v>
       </c>
       <c r="D934" s="30" t="s">
-        <v>4698</v>
+        <v>4697</v>
       </c>
       <c r="E934" s="30" t="s">
-        <v>4698</v>
+        <v>4697</v>
       </c>
       <c r="F934" s="26"/>
     </row>
@@ -39568,10 +39614,10 @@
         <v>1057</v>
       </c>
       <c r="D935" s="27" t="s">
-        <v>4769</v>
+        <v>4768</v>
       </c>
       <c r="E935" s="27" t="s">
-        <v>4699</v>
+        <v>4698</v>
       </c>
       <c r="F935" s="26"/>
     </row>
@@ -39586,10 +39632,10 @@
         <v>1057</v>
       </c>
       <c r="D936" s="27" t="s">
+        <v>4700</v>
+      </c>
+      <c r="E936" s="27" t="s">
         <v>4701</v>
-      </c>
-      <c r="E936" s="27" t="s">
-        <v>4702</v>
       </c>
       <c r="F936" s="26"/>
     </row>
@@ -39604,10 +39650,10 @@
         <v>1057</v>
       </c>
       <c r="D937" s="27" t="s">
+        <v>4702</v>
+      </c>
+      <c r="E937" s="27" t="s">
         <v>4703</v>
-      </c>
-      <c r="E937" s="27" t="s">
-        <v>4704</v>
       </c>
       <c r="F937" s="26"/>
     </row>
@@ -39622,10 +39668,10 @@
         <v>1057</v>
       </c>
       <c r="D938" s="27" t="s">
-        <v>4705</v>
+        <v>4704</v>
       </c>
       <c r="E938" s="27" t="s">
-        <v>4705</v>
+        <v>4704</v>
       </c>
       <c r="F938" s="26"/>
     </row>
@@ -39640,10 +39686,10 @@
         <v>1057</v>
       </c>
       <c r="D939" s="27" t="s">
+        <v>4705</v>
+      </c>
+      <c r="E939" s="27" t="s">
         <v>4706</v>
-      </c>
-      <c r="E939" s="27" t="s">
-        <v>4707</v>
       </c>
       <c r="F939" s="26"/>
     </row>
@@ -39658,10 +39704,10 @@
         <v>1057</v>
       </c>
       <c r="D940" s="27" t="s">
-        <v>4705</v>
+        <v>4704</v>
       </c>
       <c r="E940" s="27" t="s">
-        <v>4705</v>
+        <v>4704</v>
       </c>
       <c r="F940" s="26"/>
     </row>
@@ -39670,16 +39716,16 @@
         <v>4111</v>
       </c>
       <c r="B941" s="26" t="s">
-        <v>4770</v>
+        <v>4769</v>
       </c>
       <c r="C941" s="27" t="s">
         <v>1057</v>
       </c>
       <c r="D941" s="27" t="s">
-        <v>4771</v>
+        <v>4770</v>
       </c>
       <c r="E941" s="27" t="s">
-        <v>4708</v>
+        <v>4707</v>
       </c>
       <c r="F941" s="26"/>
     </row>
@@ -39694,10 +39740,10 @@
         <v>1057</v>
       </c>
       <c r="D942" s="27" t="s">
-        <v>4709</v>
+        <v>4708</v>
       </c>
       <c r="E942" s="27" t="s">
-        <v>4709</v>
+        <v>4708</v>
       </c>
       <c r="F942" s="26"/>
     </row>
@@ -39706,16 +39752,16 @@
         <v>4114</v>
       </c>
       <c r="B943" s="26" t="s">
-        <v>4772</v>
+        <v>4771</v>
       </c>
       <c r="C943" s="27" t="s">
         <v>1057</v>
       </c>
       <c r="D943" s="27" t="s">
-        <v>4710</v>
+        <v>4709</v>
       </c>
       <c r="E943" s="27" t="s">
-        <v>4710</v>
+        <v>4709</v>
       </c>
       <c r="F943" s="26"/>
     </row>
@@ -39730,10 +39776,10 @@
         <v>1057</v>
       </c>
       <c r="D944" s="27" t="s">
-        <v>4710</v>
+        <v>4709</v>
       </c>
       <c r="E944" s="27" t="s">
-        <v>4710</v>
+        <v>4709</v>
       </c>
       <c r="F944" s="26"/>
     </row>
@@ -39748,10 +39794,10 @@
         <v>1057</v>
       </c>
       <c r="D945" s="27" t="s">
+        <v>4710</v>
+      </c>
+      <c r="E945" s="27" t="s">
         <v>4711</v>
-      </c>
-      <c r="E945" s="27" t="s">
-        <v>4712</v>
       </c>
       <c r="F945" s="26"/>
     </row>
@@ -39766,10 +39812,10 @@
         <v>1057</v>
       </c>
       <c r="D946" s="27" t="s">
+        <v>4712</v>
+      </c>
+      <c r="E946" s="27" t="s">
         <v>4713</v>
-      </c>
-      <c r="E946" s="27" t="s">
-        <v>4714</v>
       </c>
       <c r="F946" s="26"/>
     </row>
@@ -39784,10 +39830,10 @@
         <v>1057</v>
       </c>
       <c r="D947" s="27" t="s">
-        <v>4715</v>
+        <v>4714</v>
       </c>
       <c r="E947" s="27" t="s">
-        <v>4715</v>
+        <v>4714</v>
       </c>
       <c r="F947" s="26"/>
     </row>
@@ -39814,16 +39860,16 @@
         <v>4123</v>
       </c>
       <c r="B949" s="26" t="s">
-        <v>4773</v>
+        <v>4772</v>
       </c>
       <c r="C949" s="27" t="s">
         <v>1057</v>
       </c>
       <c r="D949" s="27" t="s">
+        <v>4715</v>
+      </c>
+      <c r="E949" s="27" t="s">
         <v>4716</v>
-      </c>
-      <c r="E949" s="27" t="s">
-        <v>4717</v>
       </c>
       <c r="F949" s="26"/>
     </row>
@@ -39856,10 +39902,10 @@
         <v>1057</v>
       </c>
       <c r="D951" s="27" t="s">
-        <v>4777</v>
+        <v>4776</v>
       </c>
       <c r="E951" s="27" t="s">
-        <v>4718</v>
+        <v>4717</v>
       </c>
       <c r="F951" s="26"/>
     </row>
@@ -39874,10 +39920,10 @@
         <v>1057</v>
       </c>
       <c r="D952" s="27" t="s">
-        <v>4720</v>
+        <v>4719</v>
       </c>
       <c r="E952" s="27" t="s">
-        <v>4720</v>
+        <v>4719</v>
       </c>
       <c r="F952" s="26"/>
     </row>
@@ -39955,10 +40001,10 @@
     </row>
     <row r="957" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A957" s="25" t="s">
+        <v>4799</v>
+      </c>
+      <c r="B957" s="26" t="s">
         <v>4800</v>
-      </c>
-      <c r="B957" s="26" t="s">
-        <v>4801</v>
       </c>
       <c r="C957" s="27" t="s">
         <v>1057</v>
@@ -39973,19 +40019,19 @@
     </row>
     <row r="958" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A958" s="25" t="s">
+        <v>4794</v>
+      </c>
+      <c r="B958" s="26" t="s">
         <v>4795</v>
-      </c>
-      <c r="B958" s="26" t="s">
-        <v>4796</v>
       </c>
       <c r="C958" s="27" t="s">
         <v>1057</v>
       </c>
       <c r="D958" s="27" t="s">
-        <v>4721</v>
+        <v>4720</v>
       </c>
       <c r="E958" s="27" t="s">
-        <v>4721</v>
+        <v>4720</v>
       </c>
       <c r="F958" s="26"/>
     </row>
@@ -40000,10 +40046,10 @@
         <v>1057</v>
       </c>
       <c r="D959" s="27" t="s">
-        <v>4722</v>
+        <v>4721</v>
       </c>
       <c r="E959" s="27" t="s">
-        <v>4722</v>
+        <v>4721</v>
       </c>
       <c r="F959" s="26"/>
     </row>
@@ -40054,10 +40100,10 @@
         <v>1057</v>
       </c>
       <c r="D962" s="27" t="s">
+        <v>4724</v>
+      </c>
+      <c r="E962" s="27" t="s">
         <v>4725</v>
-      </c>
-      <c r="E962" s="27" t="s">
-        <v>4726</v>
       </c>
       <c r="F962" s="26"/>
     </row>
@@ -40072,10 +40118,10 @@
         <v>1057</v>
       </c>
       <c r="D963" s="27" t="s">
-        <v>4727</v>
+        <v>4726</v>
       </c>
       <c r="E963" s="27" t="s">
-        <v>4727</v>
+        <v>4726</v>
       </c>
       <c r="F963" s="26"/>
     </row>
@@ -40108,7 +40154,7 @@
         <v>1057</v>
       </c>
       <c r="D965" s="27" t="s">
-        <v>4728</v>
+        <v>4727</v>
       </c>
       <c r="E965" s="27" t="s">
         <v>2713</v>
@@ -40126,10 +40172,10 @@
         <v>1057</v>
       </c>
       <c r="D966" s="27" t="s">
+        <v>4728</v>
+      </c>
+      <c r="E966" s="27" t="s">
         <v>4729</v>
-      </c>
-      <c r="E966" s="27" t="s">
-        <v>4730</v>
       </c>
       <c r="F966" s="26"/>
     </row>
@@ -40138,16 +40184,16 @@
         <v>4161</v>
       </c>
       <c r="B967" s="26" t="s">
-        <v>4780</v>
+        <v>4779</v>
       </c>
       <c r="C967" s="27" t="s">
         <v>1057</v>
       </c>
       <c r="D967" s="27" t="s">
+        <v>4730</v>
+      </c>
+      <c r="E967" s="27" t="s">
         <v>4731</v>
-      </c>
-      <c r="E967" s="27" t="s">
-        <v>4732</v>
       </c>
       <c r="F967" s="26"/>
     </row>
@@ -40162,10 +40208,10 @@
         <v>1057</v>
       </c>
       <c r="D968" s="26" t="s">
+        <v>4732</v>
+      </c>
+      <c r="E968" s="26" t="s">
         <v>4733</v>
-      </c>
-      <c r="E968" s="26" t="s">
-        <v>4734</v>
       </c>
       <c r="F968" s="26"/>
     </row>
@@ -40174,16 +40220,16 @@
         <v>4162</v>
       </c>
       <c r="B969" s="26" t="s">
-        <v>4526</v>
+        <v>4525</v>
       </c>
       <c r="C969" s="27" t="s">
         <v>1057</v>
       </c>
       <c r="D969" s="27" t="s">
+        <v>4734</v>
+      </c>
+      <c r="E969" s="27" t="s">
         <v>4735</v>
-      </c>
-      <c r="E969" s="27" t="s">
-        <v>4736</v>
       </c>
       <c r="F969" s="26"/>
     </row>
@@ -40192,16 +40238,16 @@
         <v>4164</v>
       </c>
       <c r="B970" s="26" t="s">
-        <v>4528</v>
+        <v>4527</v>
       </c>
       <c r="C970" s="27" t="s">
         <v>1057</v>
       </c>
       <c r="D970" s="27" t="s">
+        <v>4736</v>
+      </c>
+      <c r="E970" s="27" t="s">
         <v>4737</v>
-      </c>
-      <c r="E970" s="27" t="s">
-        <v>4738</v>
       </c>
       <c r="F970" s="26"/>
     </row>
@@ -40210,16 +40256,16 @@
         <v>4166</v>
       </c>
       <c r="B971" s="26" t="s">
-        <v>4530</v>
+        <v>4529</v>
       </c>
       <c r="C971" s="27" t="s">
         <v>1057</v>
       </c>
       <c r="D971" s="27" t="s">
+        <v>4738</v>
+      </c>
+      <c r="E971" s="27" t="s">
         <v>4739</v>
-      </c>
-      <c r="E971" s="27" t="s">
-        <v>4740</v>
       </c>
       <c r="F971" s="26"/>
     </row>
@@ -40228,16 +40274,16 @@
         <v>4167</v>
       </c>
       <c r="B972" s="26" t="s">
-        <v>4531</v>
+        <v>4530</v>
       </c>
       <c r="C972" s="27" t="s">
         <v>1057</v>
       </c>
       <c r="D972" s="27" t="s">
+        <v>4740</v>
+      </c>
+      <c r="E972" s="27" t="s">
         <v>4741</v>
-      </c>
-      <c r="E972" s="27" t="s">
-        <v>4742</v>
       </c>
       <c r="F972" s="26"/>
     </row>
@@ -40246,7 +40292,7 @@
         <v>4172</v>
       </c>
       <c r="B973" s="26" t="s">
-        <v>4536</v>
+        <v>4535</v>
       </c>
       <c r="C973" s="27" t="s">
         <v>1057</v>
@@ -40264,16 +40310,16 @@
         <v>4181</v>
       </c>
       <c r="B974" s="26" t="s">
-        <v>4545</v>
+        <v>4544</v>
       </c>
       <c r="C974" s="27" t="s">
         <v>1057</v>
       </c>
       <c r="D974" s="27" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="E974" s="27" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="F974" s="26"/>
     </row>
@@ -40282,7 +40328,7 @@
         <v>4193</v>
       </c>
       <c r="B975" s="26" t="s">
-        <v>4556</v>
+        <v>4555</v>
       </c>
       <c r="C975" s="27" t="s">
         <v>1057</v>
@@ -40300,7 +40346,7 @@
         <v>4197</v>
       </c>
       <c r="B976" s="26" t="s">
-        <v>4560</v>
+        <v>4559</v>
       </c>
       <c r="C976" s="27" t="s">
         <v>1057</v>
@@ -40318,7 +40364,7 @@
         <v>4202</v>
       </c>
       <c r="B977" s="26" t="s">
-        <v>4565</v>
+        <v>4564</v>
       </c>
       <c r="C977" s="27" t="s">
         <v>1057</v>
@@ -40339,13 +40385,13 @@
         <v>4272</v>
       </c>
       <c r="C978" s="27" t="s">
-        <v>4588</v>
+        <v>4587</v>
       </c>
       <c r="D978" s="26" t="s">
+        <v>4750</v>
+      </c>
+      <c r="E978" s="26" t="s">
         <v>4751</v>
-      </c>
-      <c r="E978" s="26" t="s">
-        <v>4752</v>
       </c>
       <c r="F978" s="26"/>
     </row>
@@ -40357,13 +40403,13 @@
         <v>4504</v>
       </c>
       <c r="C979" s="27" t="s">
-        <v>4588</v>
+        <v>4587</v>
       </c>
       <c r="D979" s="27" t="s">
-        <v>4778</v>
+        <v>4777</v>
       </c>
       <c r="E979" s="27" t="s">
-        <v>4719</v>
+        <v>4718</v>
       </c>
       <c r="F979" s="26"/>
     </row>
@@ -40411,7 +40457,7 @@
         <v>4471</v>
       </c>
       <c r="C982" s="27" t="s">
-        <v>4591</v>
+        <v>4590</v>
       </c>
       <c r="D982" s="27" t="s">
         <v>1084</v>
@@ -40864,10 +40910,10 @@
         <v>2673</v>
       </c>
       <c r="D1007" s="26" t="s">
+        <v>4747</v>
+      </c>
+      <c r="E1007" s="26" t="s">
         <v>4748</v>
-      </c>
-      <c r="E1007" s="26" t="s">
-        <v>4749</v>
       </c>
       <c r="F1007" s="26"/>
     </row>
@@ -40918,10 +40964,10 @@
         <v>2673</v>
       </c>
       <c r="D1010" s="26" t="s">
-        <v>4748</v>
+        <v>4747</v>
       </c>
       <c r="E1010" s="26" t="s">
-        <v>4755</v>
+        <v>4754</v>
       </c>
       <c r="F1010" s="26"/>
     </row>
@@ -40969,7 +41015,7 @@
         <v>4418</v>
       </c>
       <c r="C1013" s="27" t="s">
-        <v>4589</v>
+        <v>4588</v>
       </c>
       <c r="D1013" s="27" t="s">
         <v>1084</v>
@@ -40987,7 +41033,7 @@
         <v>4500</v>
       </c>
       <c r="C1014" s="27" t="s">
-        <v>4589</v>
+        <v>4588</v>
       </c>
       <c r="D1014" s="27" t="s">
         <v>1084</v>
@@ -41005,7 +41051,7 @@
         <v>4502</v>
       </c>
       <c r="C1015" s="27" t="s">
-        <v>4589</v>
+        <v>4588</v>
       </c>
       <c r="D1015" s="27" t="s">
         <v>1084</v>
@@ -41023,7 +41069,7 @@
         <v>4503</v>
       </c>
       <c r="C1016" s="27" t="s">
-        <v>4589</v>
+        <v>4588</v>
       </c>
       <c r="D1016" s="27" t="s">
         <v>1084</v>
@@ -41041,7 +41087,7 @@
         <v>4514</v>
       </c>
       <c r="C1017" s="27" t="s">
-        <v>4589</v>
+        <v>4588</v>
       </c>
       <c r="D1017" s="27" t="s">
         <v>1084</v>
@@ -41059,25 +41105,25 @@
         <v>4518</v>
       </c>
       <c r="C1018" s="27" t="s">
-        <v>4589</v>
+        <v>4588</v>
       </c>
       <c r="D1018" s="27" t="s">
+        <v>4722</v>
+      </c>
+      <c r="E1018" s="27" t="s">
         <v>4723</v>
       </c>
-      <c r="E1018" s="27" t="s">
-        <v>4724</v>
-      </c>
       <c r="F1018" s="26"/>
     </row>
-    <row r="1019" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="1019" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A1019" s="25" t="s">
-        <v>4159</v>
+        <v>4845</v>
       </c>
       <c r="B1019" s="26" t="s">
-        <v>4524</v>
+        <v>4848</v>
       </c>
       <c r="C1019" s="27" t="s">
-        <v>4589</v>
+        <v>4588</v>
       </c>
       <c r="D1019" s="27" t="s">
         <v>1084</v>
@@ -41092,10 +41138,10 @@
         <v>4165</v>
       </c>
       <c r="B1020" s="26" t="s">
-        <v>4529</v>
+        <v>4528</v>
       </c>
       <c r="C1020" s="27" t="s">
-        <v>4589</v>
+        <v>4588</v>
       </c>
       <c r="D1020" s="27" t="s">
         <v>1084</v>
@@ -41110,16 +41156,16 @@
         <v>4223</v>
       </c>
       <c r="B1021" s="26" t="s">
-        <v>4586</v>
+        <v>4585</v>
       </c>
       <c r="C1021" s="27" t="s">
-        <v>4589</v>
+        <v>4588</v>
       </c>
       <c r="D1021" s="27" t="s">
-        <v>4744</v>
+        <v>4743</v>
       </c>
       <c r="E1021" s="27" t="s">
-        <v>4744</v>
+        <v>4743</v>
       </c>
       <c r="F1021" s="26"/>
     </row>
@@ -41326,7 +41372,7 @@
         <v>4178</v>
       </c>
       <c r="B1033" s="26" t="s">
-        <v>4542</v>
+        <v>4541</v>
       </c>
       <c r="C1033" s="27" t="s">
         <v>3447</v>
@@ -41836,10 +41882,10 @@
         <v>1115</v>
       </c>
       <c r="D1061" s="27" t="s">
+        <v>4651</v>
+      </c>
+      <c r="E1061" s="27" t="s">
         <v>4652</v>
-      </c>
-      <c r="E1061" s="27" t="s">
-        <v>4653</v>
       </c>
       <c r="F1061" s="26"/>
     </row>
@@ -41866,7 +41912,7 @@
         <v>4030</v>
       </c>
       <c r="B1063" s="26" t="s">
-        <v>4757</v>
+        <v>4756</v>
       </c>
       <c r="C1063" s="27" t="s">
         <v>1115</v>
@@ -41884,7 +41930,7 @@
         <v>4160</v>
       </c>
       <c r="B1064" s="26" t="s">
-        <v>4525</v>
+        <v>4524</v>
       </c>
       <c r="C1064" s="27" t="s">
         <v>1115</v>
@@ -42142,10 +42188,10 @@
         <v>1116</v>
       </c>
       <c r="D1078" s="26" t="s">
-        <v>4593</v>
+        <v>4592</v>
       </c>
       <c r="E1078" s="26" t="s">
-        <v>4593</v>
+        <v>4592</v>
       </c>
       <c r="F1078" s="26"/>
     </row>
@@ -42160,10 +42206,10 @@
         <v>1116</v>
       </c>
       <c r="D1079" s="24" t="s">
-        <v>4598</v>
+        <v>4597</v>
       </c>
       <c r="E1079" s="24" t="s">
-        <v>4598</v>
+        <v>4597</v>
       </c>
       <c r="F1079" s="26"/>
     </row>
@@ -42178,10 +42224,10 @@
         <v>1116</v>
       </c>
       <c r="D1080" s="26" t="s">
-        <v>4631</v>
+        <v>4630</v>
       </c>
       <c r="E1080" s="26" t="s">
-        <v>4631</v>
+        <v>4630</v>
       </c>
       <c r="F1080" s="26"/>
     </row>
@@ -42196,10 +42242,10 @@
         <v>1116</v>
       </c>
       <c r="D1081" s="27" t="s">
-        <v>4631</v>
+        <v>4630</v>
       </c>
       <c r="E1081" s="27" t="s">
-        <v>4631</v>
+        <v>4630</v>
       </c>
       <c r="F1081" s="26"/>
     </row>
@@ -42214,10 +42260,10 @@
         <v>1116</v>
       </c>
       <c r="D1082" s="27" t="s">
-        <v>4654</v>
+        <v>4653</v>
       </c>
       <c r="E1082" s="27" t="s">
-        <v>4654</v>
+        <v>4653</v>
       </c>
       <c r="F1082" s="26"/>
     </row>
@@ -42232,10 +42278,10 @@
         <v>1116</v>
       </c>
       <c r="D1083" s="27" t="s">
-        <v>4692</v>
+        <v>4691</v>
       </c>
       <c r="E1083" s="27" t="s">
-        <v>4692</v>
+        <v>4691</v>
       </c>
       <c r="F1083" s="26"/>
     </row>
@@ -42250,10 +42296,10 @@
         <v>1116</v>
       </c>
       <c r="D1084" s="27" t="s">
-        <v>4692</v>
+        <v>4691</v>
       </c>
       <c r="E1084" s="27" t="s">
-        <v>4692</v>
+        <v>4691</v>
       </c>
       <c r="F1084" s="26"/>
     </row>
@@ -42262,16 +42308,16 @@
         <v>4224</v>
       </c>
       <c r="B1085" s="26" t="s">
-        <v>4587</v>
+        <v>4586</v>
       </c>
       <c r="C1085" s="27" t="s">
         <v>1116</v>
       </c>
       <c r="D1085" s="27" t="s">
-        <v>4631</v>
+        <v>4630</v>
       </c>
       <c r="E1085" s="27" t="s">
-        <v>4631</v>
+        <v>4630</v>
       </c>
       <c r="F1085" s="26"/>
     </row>
@@ -42406,7 +42452,7 @@
         <v>4214</v>
       </c>
       <c r="B1093" s="26" t="s">
-        <v>4577</v>
+        <v>4576</v>
       </c>
       <c r="C1093" s="25" t="s">
         <v>1117</v>
@@ -42424,7 +42470,7 @@
         <v>4217</v>
       </c>
       <c r="B1094" s="26" t="s">
-        <v>4580</v>
+        <v>4579</v>
       </c>
       <c r="C1094" s="25" t="s">
         <v>1117</v>
@@ -42838,7 +42884,7 @@
         <v>4201</v>
       </c>
       <c r="B1117" s="26" t="s">
-        <v>4564</v>
+        <v>4563</v>
       </c>
       <c r="C1117" s="25" t="s">
         <v>1119</v>
@@ -42856,7 +42902,7 @@
         <v>4221</v>
       </c>
       <c r="B1118" s="26" t="s">
-        <v>4584</v>
+        <v>4583</v>
       </c>
       <c r="C1118" s="25" t="s">
         <v>1119</v>
@@ -42874,7 +42920,7 @@
         <v>4222</v>
       </c>
       <c r="B1119" s="26" t="s">
-        <v>4585</v>
+        <v>4584</v>
       </c>
       <c r="C1119" s="25" t="s">
         <v>1119</v>
@@ -44296,7 +44342,7 @@
         <v>4130</v>
       </c>
       <c r="B1198" s="26" t="s">
-        <v>4776</v>
+        <v>4775</v>
       </c>
       <c r="C1198" s="27" t="s">
         <v>1121</v>
@@ -44314,7 +44360,7 @@
         <v>4169</v>
       </c>
       <c r="B1199" s="26" t="s">
-        <v>4533</v>
+        <v>4532</v>
       </c>
       <c r="C1199" s="27" t="s">
         <v>1121</v>
@@ -44332,7 +44378,7 @@
         <v>4171</v>
       </c>
       <c r="B1200" s="26" t="s">
-        <v>4535</v>
+        <v>4534</v>
       </c>
       <c r="C1200" s="27" t="s">
         <v>1121</v>
@@ -44350,7 +44396,7 @@
         <v>4176</v>
       </c>
       <c r="B1201" s="26" t="s">
-        <v>4540</v>
+        <v>4539</v>
       </c>
       <c r="C1201" s="27" t="s">
         <v>1121</v>
@@ -44368,7 +44414,7 @@
         <v>4177</v>
       </c>
       <c r="B1202" s="26" t="s">
-        <v>4541</v>
+        <v>4540</v>
       </c>
       <c r="C1202" s="27" t="s">
         <v>1121</v>
@@ -44386,7 +44432,7 @@
         <v>4186</v>
       </c>
       <c r="B1203" s="26" t="s">
-        <v>4550</v>
+        <v>4549</v>
       </c>
       <c r="C1203" s="27" t="s">
         <v>1121</v>
@@ -44404,7 +44450,7 @@
         <v>4188</v>
       </c>
       <c r="B1204" s="26" t="s">
-        <v>4552</v>
+        <v>4551</v>
       </c>
       <c r="C1204" s="27" t="s">
         <v>1121</v>
@@ -44422,7 +44468,7 @@
         <v>4196</v>
       </c>
       <c r="B1205" s="26" t="s">
-        <v>4559</v>
+        <v>4558</v>
       </c>
       <c r="C1205" s="27" t="s">
         <v>1121</v>
@@ -44440,7 +44486,7 @@
         <v>4199</v>
       </c>
       <c r="B1206" s="26" t="s">
-        <v>4562</v>
+        <v>4561</v>
       </c>
       <c r="C1206" s="27" t="s">
         <v>1121</v>
@@ -44458,7 +44504,7 @@
         <v>4211</v>
       </c>
       <c r="B1207" s="26" t="s">
-        <v>4574</v>
+        <v>4573</v>
       </c>
       <c r="C1207" s="27" t="s">
         <v>1121</v>
@@ -44476,7 +44522,7 @@
         <v>4219</v>
       </c>
       <c r="B1208" s="26" t="s">
-        <v>4582</v>
+        <v>4581</v>
       </c>
       <c r="C1208" s="27" t="s">
         <v>1121</v>
@@ -44774,10 +44820,10 @@
         <v>3071</v>
       </c>
       <c r="D1224" s="26" t="s">
-        <v>4624</v>
+        <v>4623</v>
       </c>
       <c r="E1224" s="26" t="s">
-        <v>4624</v>
+        <v>4623</v>
       </c>
       <c r="F1224" s="26"/>
     </row>
@@ -44846,10 +44892,10 @@
         <v>3071</v>
       </c>
       <c r="D1228" s="27" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="E1228" s="27" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="F1228" s="26"/>
     </row>
@@ -45812,7 +45858,7 @@
         <v>4218</v>
       </c>
       <c r="B1282" s="26" t="s">
-        <v>4581</v>
+        <v>4580</v>
       </c>
       <c r="C1282" s="25" t="s">
         <v>1125</v>
@@ -47201,7 +47247,7 @@
         <v>4420</v>
       </c>
       <c r="C1359" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1359" s="27" t="s">
         <v>1127</v>
@@ -47219,7 +47265,7 @@
         <v>4422</v>
       </c>
       <c r="C1360" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1360" s="27" t="s">
         <v>1127</v>
@@ -47237,7 +47283,7 @@
         <v>4427</v>
       </c>
       <c r="C1361" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1361" s="27" t="s">
         <v>1127</v>
@@ -47255,7 +47301,7 @@
         <v>4428</v>
       </c>
       <c r="C1362" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1362" s="27" t="s">
         <v>1127</v>
@@ -47273,7 +47319,7 @@
         <v>4429</v>
       </c>
       <c r="C1363" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1363" s="27" t="s">
         <v>1127</v>
@@ -47291,7 +47337,7 @@
         <v>4434</v>
       </c>
       <c r="C1364" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1364" s="27" t="s">
         <v>1127</v>
@@ -47309,7 +47355,7 @@
         <v>4435</v>
       </c>
       <c r="C1365" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1365" s="27" t="s">
         <v>1127</v>
@@ -47327,7 +47373,7 @@
         <v>4436</v>
       </c>
       <c r="C1366" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1366" s="27" t="s">
         <v>1127</v>
@@ -47345,7 +47391,7 @@
         <v>4437</v>
       </c>
       <c r="C1367" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1367" s="27" t="s">
         <v>1127</v>
@@ -47363,7 +47409,7 @@
         <v>4438</v>
       </c>
       <c r="C1368" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1368" s="27" t="s">
         <v>1127</v>
@@ -47381,7 +47427,7 @@
         <v>4440</v>
       </c>
       <c r="C1369" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1369" s="27" t="s">
         <v>1127</v>
@@ -47399,7 +47445,7 @@
         <v>4450</v>
       </c>
       <c r="C1370" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1370" s="27" t="s">
         <v>1127</v>
@@ -47417,7 +47463,7 @@
         <v>4473</v>
       </c>
       <c r="C1371" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1371" s="27" t="s">
         <v>1127</v>
@@ -47435,7 +47481,7 @@
         <v>4474</v>
       </c>
       <c r="C1372" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1372" s="27" t="s">
         <v>1127</v>
@@ -47453,7 +47499,7 @@
         <v>4477</v>
       </c>
       <c r="C1373" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1373" s="27" t="s">
         <v>1127</v>
@@ -47471,7 +47517,7 @@
         <v>4478</v>
       </c>
       <c r="C1374" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1374" s="27" t="s">
         <v>1127</v>
@@ -47489,7 +47535,7 @@
         <v>4479</v>
       </c>
       <c r="C1375" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1375" s="27" t="s">
         <v>1127</v>
@@ -47507,7 +47553,7 @@
         <v>4486</v>
       </c>
       <c r="C1376" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1376" s="27" t="s">
         <v>1127</v>
@@ -47525,7 +47571,7 @@
         <v>4489</v>
       </c>
       <c r="C1377" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1377" s="27" t="s">
         <v>1127</v>
@@ -47543,7 +47589,7 @@
         <v>4491</v>
       </c>
       <c r="C1378" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1378" s="27" t="s">
         <v>1127</v>
@@ -47558,10 +47604,10 @@
         <v>4127</v>
       </c>
       <c r="B1379" s="26" t="s">
-        <v>4775</v>
+        <v>4774</v>
       </c>
       <c r="C1379" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1379" s="27" t="s">
         <v>1127</v>
@@ -47579,7 +47625,7 @@
         <v>4498</v>
       </c>
       <c r="C1380" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1380" s="27" t="s">
         <v>1127</v>
@@ -47597,7 +47643,7 @@
         <v>4506</v>
       </c>
       <c r="C1381" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1381" s="27" t="s">
         <v>1127</v>
@@ -47615,7 +47661,7 @@
         <v>4507</v>
       </c>
       <c r="C1382" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1382" s="27" t="s">
         <v>1127</v>
@@ -47633,7 +47679,7 @@
         <v>4509</v>
       </c>
       <c r="C1383" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1383" s="27" t="s">
         <v>1127</v>
@@ -47648,10 +47694,10 @@
         <v>4191</v>
       </c>
       <c r="B1384" s="26" t="s">
-        <v>4554</v>
+        <v>4553</v>
       </c>
       <c r="C1384" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1384" s="27" t="s">
         <v>1127</v>
@@ -47666,10 +47712,10 @@
         <v>4198</v>
       </c>
       <c r="B1385" s="26" t="s">
-        <v>4561</v>
+        <v>4560</v>
       </c>
       <c r="C1385" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1385" s="27" t="s">
         <v>1127</v>
@@ -47684,10 +47730,10 @@
         <v>4205</v>
       </c>
       <c r="B1386" s="26" t="s">
-        <v>4568</v>
+        <v>4567</v>
       </c>
       <c r="C1386" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1386" s="27" t="s">
         <v>1127</v>
@@ -47702,10 +47748,10 @@
         <v>4212</v>
       </c>
       <c r="B1387" s="26" t="s">
-        <v>4575</v>
+        <v>4574</v>
       </c>
       <c r="C1387" s="27" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
       <c r="D1387" s="27" t="s">
         <v>1127</v>
@@ -48188,10 +48234,10 @@
         <v>4136</v>
       </c>
       <c r="B1414" s="26" t="s">
-        <v>4779</v>
+        <v>4778</v>
       </c>
       <c r="C1414" s="27" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="D1414" s="27" t="s">
         <v>1127</v>
@@ -48206,10 +48252,10 @@
         <v>4208</v>
       </c>
       <c r="B1415" s="26" t="s">
-        <v>4571</v>
+        <v>4570</v>
       </c>
       <c r="C1415" s="27" t="s">
-        <v>4592</v>
+        <v>4591</v>
       </c>
       <c r="D1415" s="27" t="s">
         <v>1127</v>
@@ -49286,7 +49332,7 @@
         <v>4200</v>
       </c>
       <c r="B1475" s="26" t="s">
-        <v>4563</v>
+        <v>4562</v>
       </c>
       <c r="C1475" s="27" t="s">
         <v>1779</v>
@@ -49301,16 +49347,16 @@
     </row>
     <row r="1476" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A1476" s="3" t="s">
-        <v>4817</v>
+        <v>4816</v>
       </c>
       <c r="B1476" s="21" t="s">
-        <v>4820</v>
+        <v>4819</v>
       </c>
       <c r="C1476" s="3" t="s">
         <v>1057</v>
       </c>
       <c r="D1476" s="3" t="s">
-        <v>4821</v>
+        <v>4820</v>
       </c>
       <c r="E1476" s="3" t="s">
         <v>2713</v>
@@ -49324,21 +49370,21 @@
         <v>3835</v>
       </c>
       <c r="C1477" s="3" t="s">
-        <v>4588</v>
+        <v>4587</v>
       </c>
       <c r="D1477" s="3" t="s">
+        <v>4822</v>
+      </c>
+      <c r="E1477" s="3" t="s">
         <v>4823</v>
-      </c>
-      <c r="E1477" s="3" t="s">
-        <v>4824</v>
       </c>
     </row>
     <row r="1478" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1478" s="3" t="s">
-        <v>4802</v>
+        <v>4801</v>
       </c>
       <c r="B1478" s="15" t="s">
-        <v>4805</v>
+        <v>4804</v>
       </c>
       <c r="C1478" s="27" t="s">
         <v>1049</v>
@@ -49352,10 +49398,10 @@
     </row>
     <row r="1479" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1479" s="3" t="s">
+        <v>4824</v>
+      </c>
+      <c r="B1479" t="s">
         <v>4825</v>
-      </c>
-      <c r="B1479" t="s">
-        <v>4826</v>
       </c>
       <c r="C1479" s="3" t="s">
         <v>1057</v>
@@ -49369,19 +49415,36 @@
     </row>
     <row r="1480" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A1480" s="3" t="s">
+        <v>4830</v>
+      </c>
+      <c r="B1480" s="15" t="s">
         <v>4831</v>
-      </c>
-      <c r="B1480" s="15" t="s">
-        <v>4832</v>
       </c>
       <c r="C1480" s="3" t="s">
         <v>1057</v>
       </c>
       <c r="D1480" s="3" t="s">
+        <v>4834</v>
+      </c>
+      <c r="E1480" s="3" t="s">
         <v>4835</v>
       </c>
-      <c r="E1480" s="3" t="s">
-        <v>4836</v>
+    </row>
+    <row r="1481" spans="1:6" ht="29" x14ac:dyDescent="0.2">
+      <c r="A1481" s="3" t="s">
+        <v>4838</v>
+      </c>
+      <c r="B1481" s="15" t="s">
+        <v>4841</v>
+      </c>
+      <c r="C1481" s="3" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D1481" s="3" t="s">
+        <v>4621</v>
+      </c>
+      <c r="E1481" s="3" t="s">
+        <v>4622</v>
       </c>
     </row>
   </sheetData>
@@ -49397,10 +49460,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ABCEDD8-99CD-E64D-83C4-23A5F7177A3C}">
-  <dimension ref="A1:C1987"/>
+  <dimension ref="A1:C1988"/>
   <sheetViews>
-    <sheetView topLeftCell="A1462" workbookViewId="0">
-      <selection activeCell="D1484" sqref="D1484"/>
+    <sheetView topLeftCell="A1458" workbookViewId="0">
+      <selection activeCell="D1477" sqref="D1477"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -58586,7 +58649,7 @@
     </row>
     <row r="835" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A835" s="12" t="s">
-        <v>4782</v>
+        <v>4781</v>
       </c>
       <c r="B835" s="12" t="s">
         <v>2202</v>
@@ -65488,8 +65551,8 @@
       <c r="B1462" s="12" t="s">
         <v>2202</v>
       </c>
-      <c r="C1462" s="12" t="s">
-        <v>2202</v>
+      <c r="C1462" s="7">
+        <v>44022</v>
       </c>
     </row>
     <row r="1463" spans="1:3" x14ac:dyDescent="0.2">
@@ -65499,8 +65562,8 @@
       <c r="B1463" s="12" t="s">
         <v>2202</v>
       </c>
-      <c r="C1463" s="12" t="s">
-        <v>2202</v>
+      <c r="C1463" s="7">
+        <v>43936</v>
       </c>
     </row>
     <row r="1464" spans="1:3" x14ac:dyDescent="0.2">
@@ -65510,8 +65573,8 @@
       <c r="B1464" s="12" t="s">
         <v>2202</v>
       </c>
-      <c r="C1464" s="12" t="s">
-        <v>2202</v>
+      <c r="C1464" s="7">
+        <v>44118</v>
       </c>
     </row>
     <row r="1465" spans="1:3" x14ac:dyDescent="0.2">
@@ -65521,181 +65584,181 @@
       <c r="B1465" s="12" t="s">
         <v>2202</v>
       </c>
-      <c r="C1465" s="12" t="s">
-        <v>2202</v>
+      <c r="C1465" s="7">
+        <v>44043</v>
       </c>
     </row>
     <row r="1466" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1466" s="12" t="s">
-        <v>3850</v>
+        <v>4838</v>
       </c>
       <c r="B1466" s="12" t="s">
         <v>2202</v>
       </c>
-      <c r="C1466" s="12" t="s">
-        <v>2202</v>
+      <c r="C1466" s="7">
+        <v>44042</v>
       </c>
     </row>
     <row r="1467" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1467" s="12" t="s">
-        <v>3849</v>
+        <v>3850</v>
       </c>
       <c r="B1467" s="12" t="s">
         <v>2202</v>
       </c>
       <c r="C1467" s="7">
-        <v>44027</v>
+        <v>43981</v>
       </c>
     </row>
     <row r="1468" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1468" s="12" t="s">
-        <v>821</v>
-      </c>
-      <c r="B1468" s="7">
-        <v>43935</v>
+        <v>3849</v>
+      </c>
+      <c r="B1468" s="12" t="s">
+        <v>2202</v>
       </c>
       <c r="C1468" s="7">
-        <v>43935</v>
+        <v>44027</v>
       </c>
     </row>
     <row r="1469" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1469" s="12" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="B1469" s="7">
-        <v>43921</v>
+        <v>43935</v>
       </c>
       <c r="C1469" s="7">
-        <v>43921</v>
+        <v>43935</v>
       </c>
     </row>
     <row r="1470" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1470" s="12" t="s">
-        <v>3848</v>
+        <v>823</v>
       </c>
       <c r="B1470" s="7">
-        <v>44196</v>
+        <v>43921</v>
       </c>
       <c r="C1470" s="7">
-        <v>44196</v>
+        <v>43921</v>
       </c>
     </row>
     <row r="1471" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1471" s="12" t="s">
-        <v>3847</v>
+        <v>3848</v>
       </c>
       <c r="B1471" s="7">
-        <v>44043</v>
+        <v>44196</v>
       </c>
       <c r="C1471" s="7">
-        <v>44043</v>
+        <v>44196</v>
       </c>
     </row>
     <row r="1472" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1472" s="12" t="s">
-        <v>3846</v>
+        <v>3847</v>
       </c>
       <c r="B1472" s="7">
-        <v>44012</v>
+        <v>44043</v>
       </c>
       <c r="C1472" s="7">
-        <v>44012</v>
+        <v>44043</v>
       </c>
     </row>
     <row r="1473" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1473" s="12" t="s">
-        <v>3845</v>
+        <v>3846</v>
       </c>
       <c r="B1473" s="7">
-        <v>43952</v>
+        <v>44012</v>
       </c>
       <c r="C1473" s="7">
-        <v>43952</v>
+        <v>44012</v>
       </c>
     </row>
     <row r="1474" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1474" s="12" t="s">
-        <v>957</v>
-      </c>
-      <c r="B1474" s="12" t="s">
-        <v>2202</v>
+        <v>3845</v>
+      </c>
+      <c r="B1474" s="7">
+        <v>43952</v>
       </c>
       <c r="C1474" s="7">
-        <v>43900</v>
+        <v>43952</v>
       </c>
     </row>
     <row r="1475" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1475" s="12" t="s">
-        <v>3830</v>
-      </c>
-      <c r="B1475" s="7">
-        <v>44362</v>
+        <v>957</v>
+      </c>
+      <c r="B1475" s="12" t="s">
+        <v>2202</v>
       </c>
       <c r="C1475" s="7">
-        <v>44362</v>
+        <v>43900</v>
       </c>
     </row>
     <row r="1476" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1476" s="12" t="s">
-        <v>3841</v>
+        <v>3830</v>
       </c>
       <c r="B1476" s="7">
-        <v>44348</v>
+        <v>44362</v>
       </c>
       <c r="C1476" s="7">
-        <v>44348</v>
+        <v>44362</v>
       </c>
     </row>
     <row r="1477" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1477" s="12" t="s">
-        <v>4795</v>
+        <v>3841</v>
       </c>
       <c r="B1477" s="7">
-        <v>44136</v>
+        <v>44348</v>
       </c>
       <c r="C1477" s="7">
-        <v>44136</v>
+        <v>44348</v>
       </c>
     </row>
     <row r="1478" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1478" s="12" t="s">
-        <v>4802</v>
+        <v>4794</v>
       </c>
       <c r="B1478" s="7">
-        <v>43983</v>
+        <v>44136</v>
       </c>
       <c r="C1478" s="7">
-        <v>44044</v>
+        <v>44136</v>
       </c>
     </row>
     <row r="1479" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1479" s="12" t="s">
-        <v>4800</v>
+        <v>4801</v>
       </c>
       <c r="B1479" s="7">
-        <v>44013</v>
+        <v>43983</v>
       </c>
       <c r="C1479" s="7">
-        <v>44013</v>
+        <v>44044</v>
       </c>
     </row>
     <row r="1480" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1480" s="12" t="s">
-        <v>4817</v>
+        <v>4799</v>
       </c>
       <c r="B1480" s="7">
-        <v>44044</v>
+        <v>44013</v>
       </c>
       <c r="C1480" s="7">
-        <v>44044</v>
+        <v>44013</v>
       </c>
     </row>
     <row r="1481" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1481" s="12" t="s">
-        <v>4825</v>
+        <v>4816</v>
       </c>
       <c r="B1481" s="7">
-        <v>44013</v>
+        <v>44044</v>
       </c>
       <c r="C1481" s="7">
         <v>44044</v>
@@ -65703,23 +65766,41 @@
     </row>
     <row r="1482" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1482" s="12" t="s">
-        <v>4831</v>
+        <v>4824</v>
       </c>
       <c r="B1482" s="7">
+        <v>44013</v>
+      </c>
+      <c r="C1482" s="7">
+        <v>44044</v>
+      </c>
+    </row>
+    <row r="1483" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1483" s="12" t="s">
+        <v>4830</v>
+      </c>
+      <c r="B1483" s="7">
         <v>44287</v>
       </c>
-      <c r="C1482" s="7">
+      <c r="C1483" s="7">
         <v>44409</v>
       </c>
     </row>
-    <row r="1483" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1483" s="12"/>
-    </row>
     <row r="1484" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1484" s="12"/>
+      <c r="A1484" s="12" t="s">
+        <v>4845</v>
+      </c>
+      <c r="B1484" s="7">
+        <v>44135</v>
+      </c>
+      <c r="C1484" s="7">
+        <v>44287</v>
+      </c>
     </row>
     <row r="1485" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1485" s="12"/>
+      <c r="B1485" s="7"/>
+      <c r="C1485" s="7"/>
     </row>
     <row r="1486" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1486" s="12"/>
@@ -67226,6 +67307,9 @@
     </row>
     <row r="1987" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1987" s="12"/>
+    </row>
+    <row r="1988" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1988" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -67744,7 +67828,7 @@
         <v>3060</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>4808</v>
+        <v>4807</v>
       </c>
       <c r="C36" s="12" t="s">
         <v>2204</v>
@@ -67758,7 +67842,7 @@
         <v>2014</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>4809</v>
+        <v>4808</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>2204</v>
@@ -73571,9 +73655,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2897C11-45D0-1143-9B66-314A64F11CA5}">
   <dimension ref="A1:Q1048575"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -74363,7 +74447,7 @@
         <v>2771</v>
       </c>
       <c r="F16" t="s">
-        <v>4791</v>
+        <v>4790</v>
       </c>
       <c r="G16" t="s">
         <v>1797</v>
@@ -74378,16 +74462,16 @@
         <v>1808</v>
       </c>
       <c r="K16" t="s">
+        <v>4791</v>
+      </c>
+      <c r="L16" s="1" t="s">
         <v>4792</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>4793</v>
       </c>
       <c r="M16">
         <v>194</v>
       </c>
       <c r="N16" s="10" t="s">
-        <v>4794</v>
+        <v>4793</v>
       </c>
       <c r="P16" s="4">
         <v>43927</v>
@@ -74398,7 +74482,7 @@
     </row>
     <row r="17" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>4795</v>
+        <v>4794</v>
       </c>
       <c r="B17" t="s">
         <v>1796</v>
@@ -74428,16 +74512,16 @@
         <v>1808</v>
       </c>
       <c r="K17" t="s">
-        <v>4796</v>
+        <v>4795</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>4798</v>
+        <v>4797</v>
       </c>
       <c r="M17">
         <v>304</v>
       </c>
       <c r="N17" s="10" t="s">
-        <v>4797</v>
+        <v>4796</v>
       </c>
       <c r="P17" s="4">
         <v>43941</v>
@@ -74448,7 +74532,7 @@
     </row>
     <row r="18" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>4802</v>
+        <v>4801</v>
       </c>
       <c r="B18" t="s">
         <v>1796</v>
@@ -74463,7 +74547,7 @@
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>4804</v>
+        <v>4803</v>
       </c>
       <c r="G18" t="s">
         <v>1807</v>
@@ -74478,16 +74562,16 @@
         <v>1808</v>
       </c>
       <c r="K18" t="s">
+        <v>4804</v>
+      </c>
+      <c r="L18" s="1" t="s">
         <v>4805</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>4806</v>
       </c>
       <c r="M18">
         <v>138</v>
       </c>
       <c r="N18" s="10" t="s">
-        <v>4807</v>
+        <v>4806</v>
       </c>
       <c r="P18" s="4">
         <v>43945</v>
@@ -74498,7 +74582,7 @@
     </row>
     <row r="19" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>4800</v>
+        <v>4799</v>
       </c>
       <c r="B19" t="s">
         <v>1796</v>
@@ -74528,16 +74612,16 @@
         <v>1808</v>
       </c>
       <c r="K19" t="s">
-        <v>4801</v>
+        <v>4800</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>4811</v>
+        <v>4810</v>
       </c>
       <c r="M19">
         <v>260</v>
       </c>
       <c r="N19" s="10" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
       <c r="P19" s="4">
         <v>43942</v>
@@ -74548,7 +74632,7 @@
     </row>
     <row r="20" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>4817</v>
+        <v>4816</v>
       </c>
       <c r="B20" t="s">
         <v>1796</v>
@@ -74578,16 +74662,16 @@
         <v>2366</v>
       </c>
       <c r="K20" t="s">
-        <v>4820</v>
+        <v>4819</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>4819</v>
+        <v>4818</v>
       </c>
       <c r="M20">
         <v>500</v>
       </c>
       <c r="N20" s="10" t="s">
-        <v>4818</v>
+        <v>4817</v>
       </c>
       <c r="P20" s="4">
         <v>43945</v>
@@ -74598,7 +74682,7 @@
     </row>
     <row r="21" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>4825</v>
+        <v>4824</v>
       </c>
       <c r="B21" t="s">
         <v>1796</v>
@@ -74625,16 +74709,16 @@
         <v>1799</v>
       </c>
       <c r="K21" t="s">
+        <v>4825</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>4826</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>4827</v>
       </c>
       <c r="M21">
         <v>440</v>
       </c>
       <c r="N21" s="10" t="s">
-        <v>4828</v>
+        <v>4827</v>
       </c>
       <c r="P21" s="4">
         <v>43928</v>
@@ -74645,7 +74729,7 @@
     </row>
     <row r="22" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>4831</v>
+        <v>4830</v>
       </c>
       <c r="B22" t="s">
         <v>1796</v>
@@ -74675,21 +74759,121 @@
         <v>2366</v>
       </c>
       <c r="K22" t="s">
+        <v>4831</v>
+      </c>
+      <c r="L22" s="1" t="s">
         <v>4832</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>4833</v>
       </c>
       <c r="M22">
         <v>500</v>
       </c>
       <c r="N22" s="10" t="s">
-        <v>4834</v>
+        <v>4833</v>
       </c>
       <c r="P22" s="4">
         <v>43931</v>
       </c>
       <c r="Q22" s="4">
+        <v>43943</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>4838</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4839</v>
+      </c>
+      <c r="C23" s="4">
+        <v>43917</v>
+      </c>
+      <c r="D23" s="4">
+        <v>43910</v>
+      </c>
+      <c r="E23" t="b">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>4840</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1807</v>
+      </c>
+      <c r="H23" t="s">
+        <v>1803</v>
+      </c>
+      <c r="I23" t="s">
+        <v>1804</v>
+      </c>
+      <c r="J23" t="s">
+        <v>2372</v>
+      </c>
+      <c r="K23" t="s">
+        <v>4841</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>4842</v>
+      </c>
+      <c r="M23">
+        <v>6000</v>
+      </c>
+      <c r="N23" s="10" t="s">
+        <v>4843</v>
+      </c>
+      <c r="P23" s="4">
+        <v>43930</v>
+      </c>
+      <c r="Q23" s="4">
+        <v>43943</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="102" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>4845</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1796</v>
+      </c>
+      <c r="C24" s="4">
+        <v>43928</v>
+      </c>
+      <c r="D24" s="4">
+        <v>43922</v>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>3571</v>
+      </c>
+      <c r="G24" t="s">
+        <v>1797</v>
+      </c>
+      <c r="H24" t="s">
+        <v>1810</v>
+      </c>
+      <c r="I24" t="s">
+        <v>1799</v>
+      </c>
+      <c r="J24" t="s">
+        <v>4847</v>
+      </c>
+      <c r="K24" t="s">
+        <v>4848</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>4849</v>
+      </c>
+      <c r="M24">
+        <v>1000</v>
+      </c>
+      <c r="N24" s="10" t="s">
+        <v>4850</v>
+      </c>
+      <c r="P24" s="4">
+        <v>43941</v>
+      </c>
+      <c r="Q24" s="4">
         <v>43943</v>
       </c>
     </row>
@@ -74714,6 +74898,8 @@
     <hyperlink ref="N20" r:id="rId14" xr:uid="{51FCB3E7-387F-5147-BA11-3712E92D1ACE}"/>
     <hyperlink ref="N21" r:id="rId15" xr:uid="{211996B6-7C5B-C448-9DF3-8173DBE852F8}"/>
     <hyperlink ref="N22" r:id="rId16" xr:uid="{10BD727B-D2E9-EE49-9804-34B01BE50D82}"/>
+    <hyperlink ref="N23" r:id="rId17" xr:uid="{2268B2A9-4184-104E-AAD9-E48427D36758}"/>
+    <hyperlink ref="N24" r:id="rId18" xr:uid="{6A6406AA-FC72-6C41-9F2F-BDFB1098F670}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -74721,10 +74907,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5218A77D-399C-1D47-B6D8-167C71D40314}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -75061,10 +75247,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>4782</v>
+      </c>
+      <c r="B25" t="s">
         <v>4783</v>
-      </c>
-      <c r="B25" t="s">
-        <v>4784</v>
       </c>
       <c r="D25" t="s">
         <v>1796</v>
@@ -75075,7 +75261,7 @@
         <v>757</v>
       </c>
       <c r="B26" t="s">
-        <v>4785</v>
+        <v>4784</v>
       </c>
       <c r="D26" t="s">
         <v>1796</v>
@@ -75086,7 +75272,7 @@
         <v>4026</v>
       </c>
       <c r="B27" t="s">
-        <v>4786</v>
+        <v>4785</v>
       </c>
       <c r="D27" t="s">
         <v>1796</v>
@@ -75097,7 +75283,7 @@
         <v>2057</v>
       </c>
       <c r="B28" t="s">
-        <v>4787</v>
+        <v>4786</v>
       </c>
       <c r="D28" t="s">
         <v>1796</v>
@@ -75108,7 +75294,7 @@
         <v>3902</v>
       </c>
       <c r="B29" t="s">
-        <v>4788</v>
+        <v>4787</v>
       </c>
       <c r="D29" t="s">
         <v>1796</v>
@@ -75119,7 +75305,7 @@
         <v>3897</v>
       </c>
       <c r="B30" t="s">
-        <v>4789</v>
+        <v>4788</v>
       </c>
       <c r="D30" t="s">
         <v>1796</v>
@@ -75130,7 +75316,7 @@
         <v>2983</v>
       </c>
       <c r="B31" t="s">
-        <v>4790</v>
+        <v>4789</v>
       </c>
       <c r="C31" t="s">
         <v>4160</v>
@@ -75141,10 +75327,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>4800</v>
+        <v>4799</v>
       </c>
       <c r="B32" t="s">
-        <v>4799</v>
+        <v>4798</v>
       </c>
       <c r="C32" t="s">
         <v>4146</v>
@@ -75155,10 +75341,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>4801</v>
+      </c>
+      <c r="B33" t="s">
         <v>4802</v>
-      </c>
-      <c r="B33" t="s">
-        <v>4803</v>
       </c>
       <c r="C33" t="s">
         <v>4148</v>
@@ -75169,10 +75355,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>4795</v>
+        <v>4794</v>
       </c>
       <c r="B34" t="s">
-        <v>4810</v>
+        <v>4809</v>
       </c>
       <c r="C34" t="s">
         <v>4149</v>
@@ -75186,7 +75372,7 @@
         <v>2466</v>
       </c>
       <c r="B35" t="s">
-        <v>4813</v>
+        <v>4812</v>
       </c>
       <c r="D35" t="s">
         <v>1796</v>
@@ -75197,10 +75383,38 @@
         <v>2421</v>
       </c>
       <c r="B36" t="s">
-        <v>4814</v>
+        <v>4813</v>
       </c>
       <c r="D36" t="s">
         <v>2762</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>3244</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4844</v>
+      </c>
+      <c r="C37" t="s">
+        <v>2039</v>
+      </c>
+      <c r="D37" t="s">
+        <v>2760</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>4845</v>
+      </c>
+      <c r="B38" t="s">
+        <v>4846</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4159</v>
+      </c>
+      <c r="D38" t="s">
+        <v>2760</v>
       </c>
     </row>
   </sheetData>

</xml_diff>